<commit_message>
JReddy Changes upto 16Sep
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/Test.xlsx
+++ b/src/test/resources/excel/Test.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29127"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rajeena.RR\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jagadeesh.Reddy\Desktop\ipim\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDE63EC8-641D-4A7D-887E-205F81E19152}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2AFAAE7-1099-44EA-862C-39736FE85BC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="780" firstSheet="43" activeTab="48" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" tabRatio="780" firstSheet="45" activeTab="48" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AddCatalogs" sheetId="80" r:id="rId1"/>
@@ -87,7 +87,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17788" uniqueCount="1972">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17822" uniqueCount="1978">
   <si>
     <t>TestCaseName</t>
   </si>
@@ -5990,9 +5990,6 @@
     <t>GTIN</t>
   </si>
   <si>
-    <t>verify_Dimensions_iPIM_JSON_Verification_US</t>
-  </si>
-  <si>
     <t>verify_GTINAndClassCodesID_In_IPIMJson_US</t>
   </si>
   <si>
@@ -6002,7 +5999,28 @@
     <t>Pricing UOM</t>
   </si>
   <si>
-    <t>verify_Product_Description_JSON_Verification_US</t>
+    <t>verify_Dimensions_ItemCategoryID_GlobalMessageID_NonBaseCatalogToProductMapping_ItemClassification_iPIM_JSON_Verification_US</t>
+  </si>
+  <si>
+    <t>6037773</t>
+  </si>
+  <si>
+    <t>verify_Prices_JSON_Verification_US</t>
+  </si>
+  <si>
+    <t>5803430</t>
+  </si>
+  <si>
+    <t>9870464</t>
+  </si>
+  <si>
+    <t>verify_Competitor_Price_JSON_Verification_US</t>
+  </si>
+  <si>
+    <t>Alternative item no. (selling, &lt;Public&gt;)</t>
+  </si>
+  <si>
+    <t>Competitor_ACESOUTH</t>
   </si>
 </sst>
 </file>
@@ -6229,7 +6247,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="97">
+  <cellXfs count="96">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
@@ -6360,7 +6378,6 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -6659,26 +6676,26 @@
       <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="46.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="21.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="46.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="21.77734375" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="11" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="5" width="15.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="23.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="10.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="11.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="22.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="20.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="15.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="17.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="16.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="18.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="14.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="15.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="18" width="18.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="12.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="22.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="5" width="15.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="23.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="10.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="11.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="22.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="20.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="15.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="17.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="16.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="18.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="14.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="15.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="18" width="18.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="12.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="22.21875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20">
@@ -7066,21 +7083,21 @@
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="149.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="149.5546875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="11" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="17" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="17.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="6" width="11.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="17.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="14.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="20.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="27.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="255.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="5.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="11.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="21.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="17.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="6" width="11.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="17.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="14.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="20.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="27.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="255.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="5.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="11.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="21.44140625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14">
@@ -7184,47 +7201,47 @@
       <selection activeCell="S1" sqref="S1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="96" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="16.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="16.81640625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="16.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="16.77734375" customWidth="1" collapsed="1"/>
     <col min="4" max="4" width="11" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="6" width="11.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="21.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="10" width="21.1796875" customWidth="1" collapsed="1"/>
+    <col min="5" max="6" width="11.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="21.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="10" width="21.21875" customWidth="1" collapsed="1"/>
     <col min="11" max="11" width="13" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="16.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="16.453125" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="18.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="25.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="25.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="22.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="39.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="22" width="39.1796875" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="28.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="24" max="24" width="25.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="25" max="25" width="29.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="26" max="26" width="29.1796875" customWidth="1" collapsed="1"/>
-    <col min="27" max="27" width="10.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="16.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="16.44140625" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="18.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="25.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="25.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="22.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="39.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="22" width="39.21875" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="28.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="25.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="25" max="25" width="29.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="26" max="26" width="29.21875" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="10.21875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="28" max="28" width="108" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="29" max="29" width="25.54296875" customWidth="1" collapsed="1"/>
-    <col min="30" max="30" width="49.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="31" max="31" width="35.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="32" max="32" width="35.54296875" customWidth="1" collapsed="1"/>
-    <col min="33" max="33" width="132.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="34" max="35" width="27.453125" customWidth="1" collapsed="1"/>
+    <col min="29" max="29" width="25.5546875" customWidth="1" collapsed="1"/>
+    <col min="30" max="30" width="49.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="31" max="31" width="35.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="32" max="32" width="35.5546875" customWidth="1" collapsed="1"/>
+    <col min="33" max="33" width="132.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="34" max="35" width="27.44140625" customWidth="1" collapsed="1"/>
     <col min="36" max="36" width="32" customWidth="1" collapsed="1"/>
-    <col min="37" max="37" width="46.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="38" max="39" width="25.81640625" customWidth="1" collapsed="1"/>
-    <col min="40" max="40" width="32.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="41" max="41" width="47.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="42" max="43" width="35.81640625" customWidth="1" collapsed="1"/>
-    <col min="44" max="44" width="32.81640625" customWidth="1" collapsed="1"/>
-    <col min="45" max="45" width="51.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="46" max="47" width="33.453125" customWidth="1" collapsed="1"/>
-    <col min="48" max="49" width="32.81640625" customWidth="1" collapsed="1"/>
-    <col min="50" max="50" width="38.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="37" max="37" width="46.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="38" max="39" width="25.77734375" customWidth="1" collapsed="1"/>
+    <col min="40" max="40" width="32.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="41" max="41" width="47.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="42" max="43" width="35.77734375" customWidth="1" collapsed="1"/>
+    <col min="44" max="44" width="32.77734375" customWidth="1" collapsed="1"/>
+    <col min="45" max="45" width="51.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="46" max="47" width="33.44140625" customWidth="1" collapsed="1"/>
+    <col min="48" max="49" width="32.77734375" customWidth="1" collapsed="1"/>
+    <col min="50" max="50" width="38.21875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:50">
@@ -7987,7 +8004,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="1:50" ht="15.65" customHeight="1">
+    <row r="6" spans="1:50" ht="15.6" customHeight="1">
       <c r="A6" t="s">
         <v>488</v>
       </c>
@@ -12713,23 +12730,23 @@
       <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="48.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="48.21875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="11" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="21.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="13.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="8.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="7" width="12.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="8.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="14.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="11.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="7.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="8.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="11.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="9.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="21.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="17" width="11.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="21.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="13.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="8.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="7" width="12.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="8.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="14.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="11.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="7.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="8.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="11.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="9.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="21.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="17" width="11.44140625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17">
@@ -13324,31 +13341,31 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:T62"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:XFD2"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="87.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="87.44140625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="11" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="4" width="11.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="23.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="11.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="9.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="13.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="18.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="4" width="11.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="23.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="11.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="9.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="13.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="18.77734375" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="10" max="10" width="17" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="11.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="14.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="255.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="5.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="10.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="36.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="12.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="13.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="13.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="11.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="14.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="255.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="5.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="10.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="36.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="12.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="13.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="13.77734375" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="20" max="20" width="19" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
@@ -17211,28 +17228,28 @@
       <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="128.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="128.21875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="11" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="4" width="11.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="13.54296875" customWidth="1" collapsed="1"/>
+    <col min="3" max="4" width="11.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="13.5546875" customWidth="1" collapsed="1"/>
     <col min="6" max="6" width="13" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="20.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="9.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="35.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="13.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="11.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="16.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="11.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="14.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="103.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="5.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="193.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="16.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="12.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="14.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="11.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="20.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="9.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="35.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="13.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="11.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="16.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="11.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="14.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="103.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="5.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="193.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="16.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="12.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="14.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="11.5546875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21">
@@ -18031,35 +18048,35 @@
       <selection activeCell="A43" sqref="A43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="84.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="3" width="11.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="16.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="84.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="3" width="11.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="16.77734375" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="11" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="20.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="64.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="16.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="19.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="30.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="11.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="6.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="4.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="16.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="4.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="7.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="11.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="11.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="4.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="14.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="13.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="11.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="14.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="24" max="24" width="16.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="25" max="25" width="103.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="26" max="26" width="5.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="27" max="27" width="33.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="28" max="28" width="16.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="20.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="64.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="16.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="19.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="30.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="11.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="6.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="4.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="16.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="4.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="7.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="11.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="11.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="4.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="14.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="13.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="11.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="14.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="16.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="25" max="25" width="103.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="26" max="26" width="5.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="33.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="28" max="28" width="16.5546875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:28">
@@ -21346,20 +21363,20 @@
       <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="78.453125" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="13.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="4" width="11.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="23.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="11.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="13.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="11.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="16.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="11.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="14.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="103.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="12.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="78.44140625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="13.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="4" width="11.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="23.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="11.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="13.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="11.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="16.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="11.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="14.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="103.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="12.21875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14">
@@ -21684,20 +21701,20 @@
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="119.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="119.44140625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="11" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="4" width="11.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="23.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="7" width="9.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="4" width="11.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="23.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="7" width="9.77734375" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="8" max="8" width="17" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="11.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="103.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="5.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="10.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="11.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="103.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="5.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="10.21875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="13" max="13" width="8" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="10.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="10.77734375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14">
@@ -21887,27 +21904,27 @@
   <sheetPr codeName="Sheet15"/>
   <dimension ref="A1:R4"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="42.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="42.5546875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="11" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="4" width="11.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="20.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="18.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="9.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="13.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="11.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="11" width="16.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="4" width="11.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="20.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="18.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="9.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="13.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="11.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="11" width="16.77734375" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="12" max="12" width="16" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="12.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="13.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="11.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="14.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="255.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="12.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="13.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="11.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="14.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="255.5546875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18">
@@ -22148,29 +22165,29 @@
       <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="79.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="79.44140625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="11" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="4" width="17.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="4" width="17.21875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="13" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="9.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="15.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="9.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="13.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="11.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="16.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="11.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="14.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="103.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="5.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="12.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="13.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="16.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="9.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="15.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="9.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="13.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="11.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="16.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="11.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="14.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="103.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="5.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="12.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="13.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="16.77734375" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="19" max="19" width="16" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="20" max="20" width="13" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="12.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="13.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="12.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="13.21875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:22">
@@ -22319,29 +22336,29 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:W13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView topLeftCell="Q1" workbookViewId="0">
+      <selection activeCell="V17" sqref="V17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="160.81640625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="36.54296875" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="31.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="11.81640625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="160.77734375" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="36.5546875" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="31.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="11.77734375" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="20" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="48.81640625" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="32.81640625" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="41.81640625" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="48.81640625" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="39.453125" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="14.54296875" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="44.81640625" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="35.81640625" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="41.81640625" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="47.1796875" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="188.1796875" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="108.1796875" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="48.77734375" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="32.77734375" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="41.77734375" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="48.77734375" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="39.44140625" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="14.5546875" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="44.77734375" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="35.77734375" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="41.77734375" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="47.21875" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="188.21875" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="108.21875" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:23">
@@ -22707,7 +22724,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="6" spans="1:23" ht="43.5">
+    <row r="6" spans="1:23" ht="43.2">
       <c r="A6" t="s">
         <v>80</v>
       </c>
@@ -22778,7 +22795,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="7" spans="1:23" ht="43.5">
+    <row r="7" spans="1:23" ht="43.2">
       <c r="A7" t="s">
         <v>87</v>
       </c>
@@ -22849,7 +22866,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="8" spans="1:23" ht="43.5">
+    <row r="8" spans="1:23" ht="43.2">
       <c r="A8" t="s">
         <v>88</v>
       </c>
@@ -22920,7 +22937,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="9" spans="1:23" ht="43.5">
+    <row r="9" spans="1:23" ht="43.2">
       <c r="A9" t="s">
         <v>89</v>
       </c>
@@ -23204,7 +23221,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="13" spans="1:23" ht="43.5">
+    <row r="13" spans="1:23" ht="43.2">
       <c r="A13" t="s">
         <v>96</v>
       </c>
@@ -23289,22 +23306,22 @@
       <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="79.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="79.5546875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="11" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="4" width="17.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="20.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="9.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="17.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="13.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="16.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="11.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="14.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="103.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="5.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="12.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="13.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="4" width="17.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="20.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="9.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="17.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="13.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="16.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="11.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="14.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="103.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="5.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="12.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="13.21875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15">
@@ -23603,26 +23620,26 @@
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="95.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="95.77734375" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="11" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="4" width="15.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="14.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="15.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="4" width="15.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="14.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="15.21875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="7" max="7" width="10" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="31.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="13.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="11.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="16.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="13.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="11.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="14.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="22.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="5.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="9.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="11.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="16.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="31.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="13.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="11.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="16.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="13.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="11.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="14.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="22.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="5.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="9.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="11.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="16.77734375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19">
@@ -23817,17 +23834,17 @@
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="52.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="3" width="16.1796875" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="52.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="3" width="16.21875" customWidth="1" collapsed="1"/>
     <col min="4" max="4" width="11" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="6" width="11.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="22.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="16.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="21.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="18.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="16.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="6" width="11.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="22.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="16.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="21.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="18.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="16.77734375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
@@ -24159,22 +24176,22 @@
       <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="89.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="89.21875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="11" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="4" width="11.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="22.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="10.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="23.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="20.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="20.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="13.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="4" width="11.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="22.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="10.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="23.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="20.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="20.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="13.21875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="11" max="11" width="17" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="11.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="14.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="255.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="5.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="11.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="14.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="255.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="5.77734375" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="16" max="16" width="10" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
@@ -25990,55 +26007,55 @@
   <dimension ref="A1:AQ70"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A65" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="B70" sqref="B70"/>
+      <selection pane="bottomLeft" activeCell="E75" sqref="E75"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="30.81640625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="58.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="30.77734375" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="58.77734375" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="17" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="4" max="4" width="11" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="23" style="31" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="17.54296875" style="31" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="176.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="14.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="17.5546875" style="31" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="176.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="14.21875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="9" max="9" width="16" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="11.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="7.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="6.54296875" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="5.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="7.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="5.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="22.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="12.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="5.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="7.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="11.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="7.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="6.5546875" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="5.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="7.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="5.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="22.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="12.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="5.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="7.77734375" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="20" max="20" width="8" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="11.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="14.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="11.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="14.21875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="23" max="23" width="16" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="24" max="24" width="9" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="25" max="25" width="5.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="26" max="26" width="11.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="27" max="27" width="36.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="28" max="29" width="20.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="30" max="30" width="14.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="31" max="31" width="16.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="32" max="32" width="13.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="33" max="33" width="11.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="34" max="34" width="14.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="35" max="35" width="20.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="36" max="36" width="14.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="37" max="37" width="39.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="38" max="38" width="9.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="39" max="39" width="21.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="25" max="25" width="5.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="26" max="26" width="11.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="36.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="28" max="29" width="20.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="30" max="30" width="14.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="31" max="31" width="16.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="32" max="32" width="13.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="33" max="33" width="11.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="34" max="34" width="14.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="35" max="35" width="20.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="36" max="36" width="14.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="37" max="37" width="39.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="38" max="38" width="9.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="39" max="39" width="21.5546875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="40" max="40" width="12" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="41" max="41" width="12.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="42" max="42" width="9.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="43" max="43" width="10.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="41" max="41" width="12.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="42" max="42" width="9.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="43" max="43" width="10.21875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:43">
@@ -29185,7 +29202,7 @@
         <v>621</v>
       </c>
     </row>
-    <row r="25" spans="1:43" ht="14.15" customHeight="1">
+    <row r="25" spans="1:43" ht="14.1" customHeight="1">
       <c r="A25" t="s">
         <v>1151</v>
       </c>
@@ -35228,32 +35245,32 @@
       <selection activeCell="U32" sqref="U32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="79.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="12.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="38.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="9.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="38.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="21.81640625" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="17.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="41.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="34.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="64.81640625" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="15.453125" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="17.81640625" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="17.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="15" width="24.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="25.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="14.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="17.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="7.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="23.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="105.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="79.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="12.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="38.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="9.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="38.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="21.77734375" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="17.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="41.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="34.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="64.77734375" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="15.44140625" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="17.77734375" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="17.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="15" width="24.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="25.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="14.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="17.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="7.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="23.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="105.44140625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="22" max="22" width="17" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="16.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="24" max="24" width="43.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="25" max="25" width="17.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="16.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="43.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="25" max="25" width="17.77734375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26">
@@ -35576,7 +35593,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:26" ht="13" customHeight="1">
+    <row r="5" spans="1:26" ht="13.05" customHeight="1">
       <c r="A5" s="13" t="s">
         <v>1432</v>
       </c>
@@ -38151,14 +38168,14 @@
       <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="24.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="11.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="18.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="22.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="24.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="11.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="18.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="22.5546875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="13" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="11.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="11.5546875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -38216,29 +38233,29 @@
       <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="81.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="3" width="16.1796875" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="16.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="81.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="3" width="16.21875" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="16.77734375" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="11" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="6" max="6" width="11" customWidth="1"/>
-    <col min="7" max="8" width="11.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="8" width="11.44140625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="9" max="9" width="13" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="16.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="18.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="25.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="22.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="26.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="16" width="56.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="56.54296875" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="39.1796875" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="28.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="38.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="25.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="42.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="29.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="24" max="24" width="10.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="16.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="18.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="25.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="22.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="26.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="16" width="56.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="56.5546875" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="39.21875" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="28.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="38.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="25.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="42.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="29.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="10.21875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26">
@@ -39455,29 +39472,29 @@
       <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="81.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="3" width="16.1796875" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="16.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="81.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="3" width="16.21875" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="16.77734375" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="11" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="6" max="6" width="11" customWidth="1"/>
-    <col min="7" max="8" width="11.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="8" width="11.44140625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="9" max="9" width="13" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="16.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="18.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="25.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="22.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="26.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="16" width="56.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="56.54296875" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="39.1796875" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="28.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="38.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="25.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="42.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="29.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="24" max="24" width="10.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="16.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="18.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="25.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="22.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="26.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="16" width="56.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="56.5546875" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="39.21875" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="28.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="38.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="25.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="42.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="29.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="10.21875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:27">
@@ -39659,29 +39676,29 @@
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="81.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="3" width="16.1796875" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="16.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="81.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="3" width="16.21875" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="16.77734375" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="11" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="6" max="6" width="11" customWidth="1"/>
-    <col min="7" max="8" width="11.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="8" width="11.44140625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="9" max="9" width="13" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="16.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="18.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="25.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="22.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="26.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="16" width="56.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="56.54296875" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="39.1796875" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="28.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="38.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="25.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="42.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="29.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="24" max="24" width="10.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="16.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="18.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="25.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="22.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="26.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="16" width="56.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="56.5546875" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="39.21875" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="28.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="38.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="25.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="42.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="29.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="10.21875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26">
@@ -40898,11 +40915,11 @@
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="18.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="30.81640625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="14.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="18.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="30.77734375" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="14.77734375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -41072,34 +41089,34 @@
       <selection activeCell="AD7" sqref="AD7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="81.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="12.453125" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="14.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="81.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="12.44140625" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="14.77734375" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="4" max="4" width="11" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="34.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="33.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="8" width="33.81640625" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="13.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="28.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="24.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="16" width="24.453125" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="8.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="15.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="70.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="25.81640625" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="25.54296875" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="77.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="23" max="24" width="25.81640625" customWidth="1" collapsed="1"/>
-    <col min="25" max="25" width="38.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="26" max="27" width="38.453125" customWidth="1" collapsed="1"/>
-    <col min="28" max="28" width="39.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="29" max="30" width="39.1796875" customWidth="1" collapsed="1"/>
-    <col min="31" max="31" width="43.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="32" max="33" width="43.1796875" customWidth="1" collapsed="1"/>
-    <col min="34" max="34" width="27.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="35" max="35" width="40.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="34.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="33.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="8" width="33.77734375" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="13.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="28.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="24.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="16" width="24.44140625" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="8.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="15.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="70.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="25.77734375" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="25.5546875" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="77.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="23" max="24" width="25.77734375" customWidth="1" collapsed="1"/>
+    <col min="25" max="25" width="38.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="26" max="27" width="38.44140625" customWidth="1" collapsed="1"/>
+    <col min="28" max="28" width="39.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="29" max="30" width="39.21875" customWidth="1" collapsed="1"/>
+    <col min="31" max="31" width="43.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="32" max="33" width="43.21875" customWidth="1" collapsed="1"/>
+    <col min="34" max="34" width="27.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="35" max="35" width="40.44140625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:35">
@@ -43790,21 +43807,21 @@
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="145.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="10.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="14.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="16.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="145.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="10.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="14.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="16.77734375" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="11" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="11.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="17.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="17.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="17.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="11.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="17.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="17.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="17.5546875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="10" max="10" width="23" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="20.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="20.5546875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="12" max="12" width="27" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="9.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="9.77734375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13">
@@ -43984,13 +44001,13 @@
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="47" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="11.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="17.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="14.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="15.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="11.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="17.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="14.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="15.77734375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
@@ -44209,12 +44226,12 @@
       <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="53.453125" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="13.81640625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="18.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="11.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="53.44140625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="13.77734375" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="18.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="11.77734375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -44426,15 +44443,15 @@
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="39.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="11.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="14.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="14.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="16.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="17.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="18.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="39.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="11.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="14.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="14.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="16.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="17.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="18.21875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
@@ -44556,13 +44573,13 @@
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="25.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="25.5546875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="2" max="3" width="11" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="14.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="16.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="11.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="14.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="16.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="11.77734375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -44618,20 +44635,20 @@
       <selection activeCell="B22" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="26.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="88.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="26.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="88.44140625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="17" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="11.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="11.77734375" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="17" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="11.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="10" width="18.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="15.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="23.90625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="31.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="15.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="75.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="11.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="10" width="18.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="15.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="23.88671875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="31.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="15.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="75.5546875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17">
@@ -45336,20 +45353,20 @@
       <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="26.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="88.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="26.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="88.44140625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="17" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="11.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="11.77734375" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="17" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="11.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="10" width="18.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="15.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="23.90625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="31.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="15.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="75.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="11.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="10" width="18.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="15.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="23.88671875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="31.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="15.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="75.5546875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17">
@@ -45524,17 +45541,17 @@
       <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="109.81640625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="18.453125" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="39.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="109.77734375" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="18.44140625" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="39.21875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="4" max="4" width="15" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="30.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="34.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="18.1796875" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="16.81640625" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="16.1796875" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="30.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="34.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="18.21875" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="16.77734375" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="16.21875" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -45569,7 +45586,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="16.5">
+    <row r="2" spans="1:10" ht="16.8">
       <c r="A2" t="s">
         <v>1786</v>
       </c>
@@ -45711,21 +45728,21 @@
       <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="80.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="80.5546875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="11" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="16.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="16.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="15.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="21.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="14.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="9.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="14.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="21.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="16.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="16.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="15.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="21.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="14.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="9.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="14.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="21.77734375" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="15" max="15" width="16" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="14.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="14.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="14.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="14.77734375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18">
@@ -46246,72 +46263,72 @@
       <selection activeCell="BF8" sqref="BF8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="84.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="11.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="17.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="40.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="15.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="11.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="84.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="11.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="17.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="40.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="15.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="11.5546875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="7" max="7" width="13" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="15.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="12.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="15.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="12.44140625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="10" max="10" width="12" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="17.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="51.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="17.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="51.44140625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="13" max="13" width="15" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="10.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="11.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="3.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="15.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="17.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="28.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="23.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="18.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="28.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="25.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="24" max="24" width="12.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="25" max="25" width="3.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="10.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="11.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="3.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="15.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="17.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="28.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="23.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="18.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="28.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="25.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="12.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="25" max="25" width="3.77734375" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="26" max="26" width="7" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="27" max="27" width="9.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="28" max="28" width="17.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="29" max="29" width="5.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="9.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="28" max="28" width="17.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="29" max="29" width="5.5546875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="30" max="30" width="10" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="31" max="31" width="12.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="32" max="32" width="11.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="33" max="33" width="16.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="34" max="34" width="7.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="35" max="35" width="10.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="36" max="36" width="4.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="31" max="31" width="12.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="32" max="32" width="11.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="33" max="33" width="16.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="34" max="34" width="7.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="35" max="35" width="10.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="36" max="36" width="4.77734375" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="37" max="37" width="9" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="38" max="38" width="6.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="39" max="39" width="11.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="40" max="40" width="7.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="41" max="41" width="11.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="42" max="42" width="13.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="38" max="38" width="6.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="39" max="39" width="11.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="40" max="40" width="7.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="41" max="41" width="11.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="42" max="42" width="13.44140625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="43" max="43" width="14" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="44" max="44" width="13.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="45" max="45" width="7.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="46" max="46" width="13.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="44" max="44" width="13.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="45" max="45" width="7.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="46" max="46" width="13.21875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="48" max="48" width="10" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="49" max="49" width="5.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="50" max="50" width="6.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="51" max="51" width="7.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="52" max="52" width="9.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="53" max="53" width="10.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="54" max="54" width="14.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="49" max="49" width="5.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="50" max="50" width="6.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="51" max="51" width="7.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="52" max="52" width="9.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="53" max="53" width="10.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="54" max="54" width="14.77734375" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="55" max="55" width="20" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="56" max="56" width="8.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="57" max="57" width="8.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="58" max="60" width="19.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="61" max="61" width="12.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="62" max="62" width="10.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="63" max="63" width="24.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="64" max="64" width="15.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="65" max="65" width="24.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="66" max="66" width="16.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="67" max="67" width="5.81640625" customWidth="1" collapsed="1"/>
+    <col min="56" max="56" width="8.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="57" max="57" width="8.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="58" max="60" width="19.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="61" max="61" width="12.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="62" max="62" width="10.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="63" max="63" width="24.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="64" max="64" width="15.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="65" max="65" width="24.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="66" max="66" width="16.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="67" max="67" width="5.77734375" customWidth="1" collapsed="1"/>
     <col min="68" max="70" width="13" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
@@ -49310,15 +49327,15 @@
       <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="19.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="19.77734375" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="11" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="11.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="17.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="7.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="14.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="15.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="11.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="17.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="7.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="14.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="15.77734375" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="8" max="8" width="17" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
@@ -49387,26 +49404,26 @@
       <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="77.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="77.5546875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="11" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="12.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="14.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="20.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="12.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="14.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="20.5546875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="6" max="6" width="10" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="8" width="18.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="8" width="18.5546875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="9" max="9" width="18" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="10" max="10" width="19" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="21.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="8.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="15.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="11.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="16.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="20.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="16.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="21.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="8.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="15.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="11.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="16.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="20.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="16.77734375" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="18" max="18" width="16" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="13.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="13.21875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19">
@@ -50073,14 +50090,14 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="74" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="11.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="11.44140625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="11" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="4" max="4" width="13" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="9.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="10.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="9.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="10.21875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -50256,17 +50273,17 @@
       <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="113.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="113.21875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="11" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="11.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="14.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="6" width="9.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="11.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="14.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="6" width="9.77734375" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="7" max="7" width="17" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="11.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="10" width="17.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="38.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="11.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="10" width="17.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="38.5546875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
@@ -50458,19 +50475,19 @@
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="83.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="11.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="21.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="29.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="21.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="25.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="15.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="83.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="11.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="21.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="29.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="21.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="25.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="15.5546875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="8" max="8" width="11" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="197.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="10.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="19.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="197.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="10.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="19.77734375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
@@ -50767,20 +50784,20 @@
       <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="85.1796875" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="21.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="11.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="24.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="16.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="17.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="11.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="85.21875" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="21.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="11.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="24.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="16.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="17.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="11.77734375" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="8" max="8" width="11" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="33.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="8.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="28.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="15.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="33.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="8.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="28.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="15.5546875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
@@ -51823,9 +51840,9 @@
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="57.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="57.5546875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -51861,20 +51878,20 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="67.1796875" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="24.1796875" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="24.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="18.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="24.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="19.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="67.21875" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="24.21875" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="24.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="18.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="24.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="19.21875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="7" max="7" width="16" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="255.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="255.77734375" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="10" max="10" width="18" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="11.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="15.453125" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="25.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="11.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="15.44140625" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="25.77734375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16">
@@ -52491,9 +52508,9 @@
       <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="19.1796875" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="19.21875" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="79.54296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="79.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -52600,21 +52617,22 @@
 
 <file path=xl/worksheets/sheet49.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2F00-000000000000}">
-  <dimension ref="A1:AH8"/>
+  <dimension ref="A1:AH9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="41.36328125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.36328125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.54296875" customWidth="1"/>
+    <col min="1" max="1" width="52.21875" customWidth="1"/>
+    <col min="6" max="6" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.5546875" customWidth="1"/>
     <col min="17" max="17" width="13" customWidth="1"/>
-    <col min="27" max="27" width="10.54296875" bestFit="1" customWidth="1"/>
-    <col min="31" max="33" width="12.6328125" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="19.6328125" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="31" max="33" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="19.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:34">
@@ -52712,7 +52730,7 @@
         <v>440</v>
       </c>
       <c r="AF1" s="11" t="s">
-        <v>1969</v>
+        <v>1968</v>
       </c>
       <c r="AG1" s="11" t="s">
         <v>441</v>
@@ -52816,7 +52834,7 @@
         <v>1958</v>
       </c>
       <c r="AF2" s="11" t="s">
-        <v>1970</v>
+        <v>1969</v>
       </c>
       <c r="AG2" s="11" t="s">
         <v>1958</v>
@@ -52920,7 +52938,7 @@
         <v>1958</v>
       </c>
       <c r="AF3" s="11" t="s">
-        <v>1970</v>
+        <v>1969</v>
       </c>
       <c r="AG3" s="11" t="s">
         <v>1958</v>
@@ -53024,7 +53042,7 @@
         <v>1958</v>
       </c>
       <c r="AF4" s="11" t="s">
-        <v>1970</v>
+        <v>1969</v>
       </c>
       <c r="AG4" s="11" t="s">
         <v>1958</v>
@@ -53128,7 +53146,7 @@
         <v>1958</v>
       </c>
       <c r="AF5" s="11" t="s">
-        <v>1970</v>
+        <v>1969</v>
       </c>
       <c r="AG5" s="11" t="s">
         <v>1958</v>
@@ -53139,7 +53157,7 @@
     </row>
     <row r="6" spans="1:34">
       <c r="A6" s="91" t="s">
-        <v>1968</v>
+        <v>1967</v>
       </c>
       <c r="B6" s="92" t="s">
         <v>106</v>
@@ -53232,7 +53250,7 @@
         <v>1966</v>
       </c>
       <c r="AF6" s="11" t="s">
-        <v>1970</v>
+        <v>1969</v>
       </c>
       <c r="AG6" s="11" t="s">
         <v>1966</v>
@@ -53243,7 +53261,7 @@
     </row>
     <row r="7" spans="1:34">
       <c r="A7" s="91" t="s">
-        <v>1967</v>
+        <v>1970</v>
       </c>
       <c r="B7" s="92" t="s">
         <v>106</v>
@@ -53261,7 +53279,7 @@
         <v>82</v>
       </c>
       <c r="G7" s="94" t="s">
-        <v>1950</v>
+        <v>1973</v>
       </c>
       <c r="H7" s="95" t="s">
         <v>24</v>
@@ -53327,7 +53345,7 @@
         <v>752</v>
       </c>
       <c r="AC7" s="93" t="s">
-        <v>1752</v>
+        <v>17</v>
       </c>
       <c r="AD7" s="93" t="s">
         <v>1752</v>
@@ -53336,7 +53354,7 @@
         <v>1958</v>
       </c>
       <c r="AF7" s="11" t="s">
-        <v>1970</v>
+        <v>1969</v>
       </c>
       <c r="AG7" s="11" t="s">
         <v>1958</v>
@@ -53346,8 +53364,8 @@
       </c>
     </row>
     <row r="8" spans="1:34">
-      <c r="A8" s="96" t="s">
-        <v>1971</v>
+      <c r="A8" s="91" t="s">
+        <v>1972</v>
       </c>
       <c r="B8" s="92" t="s">
         <v>106</v>
@@ -53365,7 +53383,7 @@
         <v>82</v>
       </c>
       <c r="G8" s="94" t="s">
-        <v>1950</v>
+        <v>1971</v>
       </c>
       <c r="H8" s="95" t="s">
         <v>24</v>
@@ -53425,7 +53443,7 @@
         <v>26</v>
       </c>
       <c r="AA8" s="93" t="s">
-        <v>1946</v>
+        <v>1944</v>
       </c>
       <c r="AB8" s="93" t="s">
         <v>1944</v>
@@ -53437,19 +53455,124 @@
         <v>1752</v>
       </c>
       <c r="AE8" s="11" t="s">
-        <v>224</v>
+        <v>1958</v>
       </c>
       <c r="AF8" s="11" t="s">
-        <v>1970</v>
+        <v>1969</v>
       </c>
       <c r="AG8" s="11" t="s">
-        <v>224</v>
+        <v>1958</v>
       </c>
       <c r="AH8" s="11" t="s">
         <v>1959</v>
       </c>
     </row>
+    <row r="9" spans="1:34">
+      <c r="A9" s="91" t="s">
+        <v>1975</v>
+      </c>
+      <c r="B9" s="92" t="s">
+        <v>106</v>
+      </c>
+      <c r="C9" s="92" t="s">
+        <v>107</v>
+      </c>
+      <c r="D9" s="93" t="s">
+        <v>34</v>
+      </c>
+      <c r="E9" s="93" t="s">
+        <v>35</v>
+      </c>
+      <c r="F9" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="G9" s="94" t="s">
+        <v>1974</v>
+      </c>
+      <c r="H9" s="95" t="s">
+        <v>24</v>
+      </c>
+      <c r="I9" s="93" t="s">
+        <v>349</v>
+      </c>
+      <c r="J9" s="93" t="s">
+        <v>26</v>
+      </c>
+      <c r="K9" s="93" t="s">
+        <v>26</v>
+      </c>
+      <c r="L9" s="93" t="s">
+        <v>26</v>
+      </c>
+      <c r="M9" s="93" t="s">
+        <v>26</v>
+      </c>
+      <c r="N9" s="93" t="s">
+        <v>26</v>
+      </c>
+      <c r="O9" s="93" t="s">
+        <v>26</v>
+      </c>
+      <c r="P9" s="93" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q9" s="11" t="s">
+        <v>398</v>
+      </c>
+      <c r="R9" s="93" t="s">
+        <v>1938</v>
+      </c>
+      <c r="S9" s="93" t="s">
+        <v>26</v>
+      </c>
+      <c r="T9" s="11" t="s">
+        <v>398</v>
+      </c>
+      <c r="U9" s="93" t="s">
+        <v>1937</v>
+      </c>
+      <c r="V9" s="11" t="s">
+        <v>398</v>
+      </c>
+      <c r="W9" s="93" t="s">
+        <v>1939</v>
+      </c>
+      <c r="X9" s="93" t="s">
+        <v>353</v>
+      </c>
+      <c r="Y9" s="93" t="s">
+        <v>26</v>
+      </c>
+      <c r="Z9" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="AA9" s="93" t="s">
+        <v>1946</v>
+      </c>
+      <c r="AB9" s="93" t="s">
+        <v>1944</v>
+      </c>
+      <c r="AC9" s="93" t="s">
+        <v>1752</v>
+      </c>
+      <c r="AD9" s="93" t="s">
+        <v>1752</v>
+      </c>
+      <c r="AE9" s="11" t="s">
+        <v>1976</v>
+      </c>
+      <c r="AF9" s="11" t="s">
+        <v>1969</v>
+      </c>
+      <c r="AG9" s="11" t="s">
+        <v>1976</v>
+      </c>
+      <c r="AH9" s="11" t="s">
+        <v>1977</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -53459,79 +53582,79 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:BW35"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="78.453125" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="11.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="17.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="25.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="15.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="11.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="78.44140625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="11.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="17.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="25.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="15.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="11.5546875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="7" max="7" width="13" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="15.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="12.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="15.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="12.44140625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="10" max="10" width="12" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="17.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="15" width="17.1796875" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="17.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="15" width="17.21875" customWidth="1" collapsed="1"/>
     <col min="16" max="16" width="25" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="17.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="17.21875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="18" max="19" width="15" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="10.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="11.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="4.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="15.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="24" max="24" width="17.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="25" max="25" width="28.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="26" max="26" width="23.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="27" max="27" width="18.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="28" max="28" width="28.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="29" max="29" width="25.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="30" max="30" width="12.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="31" max="31" width="3.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="10.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="11.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="4.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="15.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="17.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="25" max="25" width="28.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="26" max="26" width="23.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="18.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="28" max="28" width="28.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="29" max="29" width="25.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="30" max="30" width="12.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="31" max="31" width="3.77734375" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="32" max="32" width="7" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="33" max="33" width="9.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="34" max="34" width="17.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="35" max="35" width="5.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="33" max="33" width="9.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="34" max="34" width="17.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="35" max="35" width="5.5546875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="36" max="36" width="10" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="37" max="37" width="12.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="38" max="38" width="11.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="39" max="39" width="16.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="40" max="40" width="7.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="41" max="41" width="10.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="42" max="42" width="4.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="37" max="37" width="12.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="38" max="38" width="11.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="39" max="39" width="16.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="40" max="40" width="7.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="41" max="41" width="10.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="42" max="42" width="4.77734375" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="43" max="43" width="9" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="44" max="44" width="6.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="45" max="45" width="11.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="46" max="46" width="7.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="47" max="47" width="11.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="48" max="48" width="13.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="44" max="44" width="6.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="45" max="45" width="11.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="46" max="46" width="7.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="47" max="47" width="11.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="48" max="48" width="13.44140625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="49" max="49" width="14" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="50" max="50" width="13.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="51" max="51" width="7.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="52" max="52" width="13.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="53" max="53" width="9.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="50" max="50" width="13.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="51" max="51" width="7.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="52" max="52" width="13.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="53" max="53" width="9.21875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="54" max="54" width="10" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="55" max="55" width="5.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="56" max="56" width="6.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="57" max="57" width="7.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="58" max="58" width="9.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="59" max="59" width="10.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="60" max="60" width="12.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="61" max="61" width="27.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="62" max="63" width="11.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="64" max="66" width="19.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="67" max="67" width="12.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="68" max="68" width="10.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="69" max="69" width="22.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="70" max="70" width="13.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="71" max="71" width="15.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="72" max="73" width="24.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="55" max="55" width="5.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="56" max="56" width="6.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="57" max="57" width="7.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="58" max="58" width="9.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="59" max="59" width="10.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="60" max="60" width="12.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="61" max="61" width="27.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="62" max="63" width="11.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="64" max="66" width="19.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="67" max="67" width="12.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="68" max="68" width="10.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="69" max="69" width="22.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="70" max="70" width="13.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="71" max="71" width="15.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="72" max="73" width="24.77734375" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="74" max="74" width="14" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="75" max="75" width="14.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="75" max="75" width="14.21875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:71">
@@ -54006,7 +54129,7 @@
       </c>
       <c r="N3" t="str">
         <f t="shared" ref="N3:N4" ca="1" si="0">CONCATENATE(E3," ",TEXT(TODAY(),"mm-dd-yyyy"))</f>
-        <v>SICA 09-05-2025</v>
+        <v>SICA 09-16-2025</v>
       </c>
       <c r="O3" t="s">
         <v>202</v>
@@ -54222,7 +54345,7 @@
       </c>
       <c r="N4" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>MICA 09-05-2025</v>
+        <v>MICA 09-16-2025</v>
       </c>
       <c r="O4" t="s">
         <v>202</v>
@@ -61107,7 +61230,7 @@
       <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
@@ -61132,15 +61255,15 @@
       <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="51.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="5" width="15.54296875" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="16.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="14.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="13.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="25.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="25.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="51.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="5" width="15.5546875" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="16.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="14.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="13.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="25.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="25.44140625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="16" max="16" width="22" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
@@ -61258,43 +61381,43 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="64" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="17.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="13.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="14.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="16.54296875" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="43.81640625" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="16.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="6.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="11.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="5.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="11.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="17.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="13.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="14.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="16.5546875" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="43.77734375" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="16.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="6.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="11.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="5.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="11.77734375" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="13" max="13" width="17" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="14" max="14" width="11" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="13.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="17" width="11.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="13.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="17" width="11.44140625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="18" max="18" width="15" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="13.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="11.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="21" max="23" width="13.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="25" max="25" width="11.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="26" max="26" width="57.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="27" max="27" width="19.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="28" max="28" width="18.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="29" max="29" width="25.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="30" max="30" width="9.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="31" max="31" width="11.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="32" max="32" width="36.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="33" max="33" width="31.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="34" max="34" width="16.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="13.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="11.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="23" width="13.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="25" max="25" width="11.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="26" max="26" width="57.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="19.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="28" max="28" width="18.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="29" max="29" width="25.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="30" max="30" width="9.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="31" max="31" width="11.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="32" max="32" width="36.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="33" max="33" width="31.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="34" max="34" width="16.77734375" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="35" max="35" width="14" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="36" max="36" width="14.81640625" customWidth="1" collapsed="1"/>
-    <col min="37" max="37" width="15.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="38" max="38" width="11.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="36" max="36" width="14.77734375" customWidth="1" collapsed="1"/>
+    <col min="37" max="37" width="15.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="38" max="38" width="11.5546875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="39" max="39" width="13" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="40" max="40" width="11.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="40" max="40" width="11.5546875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="41" max="41" width="13" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
@@ -62812,49 +62935,49 @@
       <selection activeCell="AN10" sqref="AN10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="35.453125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.81640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.1796875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.1796875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.81640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.81640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.81640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="6.81640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.81640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="6.54296875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.81640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.54296875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="18.1796875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="35.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.21875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.21875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.77734375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.77734375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.77734375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.77734375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.77734375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="6.5546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.77734375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="18.21875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.77734375" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="13" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="25.453125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="10.54296875" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="16.1796875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="14.1796875" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="11.1796875" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="10.1796875" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="11.1796875" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="14.453125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="25.44140625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="16.21875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="14.21875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="11.21875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="10.21875" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="11.21875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="14.44140625" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="11" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="9.1796875" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="18.54296875" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="20.81640625" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="19.453125" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="27.1796875" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="10.54296875" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="12.1796875" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="38.54296875" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="33.54296875" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="22.1796875" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="9.21875" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="18.5546875" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="20.77734375" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="19.44140625" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="27.21875" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="12.21875" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="38.5546875" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="33.5546875" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="22.21875" bestFit="1" customWidth="1"/>
     <col min="35" max="35" width="15" bestFit="1" customWidth="1"/>
     <col min="36" max="36" width="16" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="16.81640625" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="12.54296875" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="12.81640625" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="22.1796875" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="17.1796875" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="16.77734375" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="12.77734375" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="22.21875" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="17.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:41">

</xml_diff>

<commit_message>
Rajeena Changes till 17Sep
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/Test.xlsx
+++ b/src/test/resources/excel/Test.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jagadeesh.Reddy\Desktop\ipim\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rajeena.RR\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2AFAAE7-1099-44EA-862C-39736FE85BC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABA6644E-A84F-41D3-A7FF-C94092F99767}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" tabRatio="780" firstSheet="45" activeTab="48" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="780" firstSheet="43" activeTab="48" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AddCatalogs" sheetId="80" r:id="rId1"/>
@@ -87,7 +87,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17822" uniqueCount="1978">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17822" uniqueCount="1975">
   <si>
     <t>TestCaseName</t>
   </si>
@@ -5990,6 +5990,9 @@
     <t>GTIN</t>
   </si>
   <si>
+    <t>verify_Dimensions_iPIM_JSON_Verification_US</t>
+  </si>
+  <si>
     <t>verify_GTINAndClassCodesID_In_IPIMJson_US</t>
   </si>
   <si>
@@ -5999,28 +6002,16 @@
     <t>Pricing UOM</t>
   </si>
   <si>
-    <t>verify_Dimensions_ItemCategoryID_GlobalMessageID_NonBaseCatalogToProductMapping_ItemClassification_iPIM_JSON_Verification_US</t>
-  </si>
-  <si>
-    <t>6037773</t>
-  </si>
-  <si>
-    <t>verify_Prices_JSON_Verification_US</t>
-  </si>
-  <si>
-    <t>5803430</t>
-  </si>
-  <si>
-    <t>9870464</t>
-  </si>
-  <si>
-    <t>verify_Competitor_Price_JSON_Verification_US</t>
-  </si>
-  <si>
-    <t>Alternative item no. (selling, &lt;Public&gt;)</t>
-  </si>
-  <si>
-    <t>Competitor_ACESOUTH</t>
+    <t>verify_Product_Description_JSON_Verification_US</t>
+  </si>
+  <si>
+    <t>verify_Product_Media_JSON_Verification_US</t>
+  </si>
+  <si>
+    <t>Media</t>
+  </si>
+  <si>
+    <t>5803732</t>
   </si>
 </sst>
 </file>
@@ -6247,7 +6238,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="96">
+  <cellXfs count="97">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
@@ -6378,6 +6369,7 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -6676,26 +6668,26 @@
       <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="46.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="21.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="46.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="21.81640625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="11" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="5" width="15.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="23.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="10.21875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="11.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="22.21875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="20.77734375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="15.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="17.21875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="16.77734375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="18.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="14.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="15.77734375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="18" width="18.77734375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="12.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="22.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="5" width="15.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="23.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="10.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="11.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="22.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="20.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="15.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="17.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="16.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="18.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="14.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="15.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="18" width="18.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="12.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="22.1796875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20">
@@ -7083,21 +7075,21 @@
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="149.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="149.54296875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="11" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="17" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="17.21875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="6" width="11.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="17.21875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="14.77734375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="20.21875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="27.77734375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="255.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="5.77734375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="11.77734375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="21.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="17.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="6" width="11.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="17.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="14.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="20.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="27.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="255.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="5.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="11.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="21.453125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14">
@@ -7201,47 +7193,47 @@
       <selection activeCell="S1" sqref="S1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="96" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="16.77734375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="16.77734375" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="16.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="16.81640625" customWidth="1" collapsed="1"/>
     <col min="4" max="4" width="11" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="6" width="11.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="21.21875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="10" width="21.21875" customWidth="1" collapsed="1"/>
+    <col min="5" max="6" width="11.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="21.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="10" width="21.1796875" customWidth="1" collapsed="1"/>
     <col min="11" max="11" width="13" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="16.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="16.44140625" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="18.77734375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="25.21875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="25.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="22.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="39.21875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="22" width="39.21875" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="28.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="24" max="24" width="25.21875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="25" max="25" width="29.21875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="26" max="26" width="29.21875" customWidth="1" collapsed="1"/>
-    <col min="27" max="27" width="10.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="16.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="16.453125" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="18.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="25.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="25.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="22.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="39.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="22" width="39.1796875" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="28.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="25.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="25" max="25" width="29.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="26" max="26" width="29.1796875" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="10.1796875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="28" max="28" width="108" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="29" max="29" width="25.5546875" customWidth="1" collapsed="1"/>
-    <col min="30" max="30" width="49.21875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="31" max="31" width="35.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="32" max="32" width="35.5546875" customWidth="1" collapsed="1"/>
-    <col min="33" max="33" width="132.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="34" max="35" width="27.44140625" customWidth="1" collapsed="1"/>
+    <col min="29" max="29" width="25.54296875" customWidth="1" collapsed="1"/>
+    <col min="30" max="30" width="49.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="31" max="31" width="35.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="32" max="32" width="35.54296875" customWidth="1" collapsed="1"/>
+    <col min="33" max="33" width="132.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="34" max="35" width="27.453125" customWidth="1" collapsed="1"/>
     <col min="36" max="36" width="32" customWidth="1" collapsed="1"/>
-    <col min="37" max="37" width="46.77734375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="38" max="39" width="25.77734375" customWidth="1" collapsed="1"/>
-    <col min="40" max="40" width="32.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="41" max="41" width="47.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="42" max="43" width="35.77734375" customWidth="1" collapsed="1"/>
-    <col min="44" max="44" width="32.77734375" customWidth="1" collapsed="1"/>
-    <col min="45" max="45" width="51.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="46" max="47" width="33.44140625" customWidth="1" collapsed="1"/>
-    <col min="48" max="49" width="32.77734375" customWidth="1" collapsed="1"/>
-    <col min="50" max="50" width="38.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="37" max="37" width="46.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="38" max="39" width="25.81640625" customWidth="1" collapsed="1"/>
+    <col min="40" max="40" width="32.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="41" max="41" width="47.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="42" max="43" width="35.81640625" customWidth="1" collapsed="1"/>
+    <col min="44" max="44" width="32.81640625" customWidth="1" collapsed="1"/>
+    <col min="45" max="45" width="51.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="46" max="47" width="33.453125" customWidth="1" collapsed="1"/>
+    <col min="48" max="49" width="32.81640625" customWidth="1" collapsed="1"/>
+    <col min="50" max="50" width="38.1796875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:50">
@@ -8004,7 +7996,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="1:50" ht="15.6" customHeight="1">
+    <row r="6" spans="1:50" ht="15.65" customHeight="1">
       <c r="A6" t="s">
         <v>488</v>
       </c>
@@ -12730,23 +12722,23 @@
       <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="48.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="48.1796875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="11" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="21.77734375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="13.77734375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="8.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="7" width="12.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="8.77734375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="14.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="11.21875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="7.77734375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="8.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="11.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="9.77734375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="21.77734375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="17" width="11.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="21.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="13.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="8.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="7" width="12.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="8.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="14.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="11.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="7.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="8.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="11.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="9.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="21.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="17" width="11.453125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17">
@@ -13341,31 +13333,31 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:T62"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A27" sqref="A27"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" sqref="A1:XFD2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="87.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="87.453125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="11" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="4" width="11.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="23.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="11.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="9.77734375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="13.21875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="18.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="4" width="11.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="23.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="11.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="9.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="13.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="18.81640625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="10" max="10" width="17" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="11.77734375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="14.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="255.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="5.77734375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="10.21875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="36.21875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="12.21875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="13.21875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="13.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="11.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="14.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="255.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="5.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="10.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="36.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="12.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="13.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="13.81640625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="20" max="20" width="19" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
@@ -17228,28 +17220,28 @@
       <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="128.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="128.1796875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="11" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="4" width="11.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="13.5546875" customWidth="1" collapsed="1"/>
+    <col min="3" max="4" width="11.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="13.54296875" customWidth="1" collapsed="1"/>
     <col min="6" max="6" width="13" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="20.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="9.77734375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="35.77734375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="13.21875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="11.77734375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="16.77734375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="11.77734375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="14.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="103.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="5.77734375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="193.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="16.77734375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="12.21875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="14.21875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="11.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="20.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="9.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="35.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="13.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="11.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="16.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="11.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="14.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="103.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="5.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="193.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="16.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="12.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="14.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="11.54296875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21">
@@ -18048,35 +18040,35 @@
       <selection activeCell="A43" sqref="A43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="84.21875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="3" width="11.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="16.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="84.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="3" width="11.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="16.81640625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="11" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="20.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="64.77734375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="16.21875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="19.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="30.21875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="11.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="6.77734375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="4.21875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="16.21875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="4.21875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="7.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="11.77734375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="11.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="4.21875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="14.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="13.21875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="11.77734375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="14.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="24" max="24" width="16.77734375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="25" max="25" width="103.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="26" max="26" width="5.77734375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="27" max="27" width="33.77734375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="28" max="28" width="16.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="20.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="64.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="16.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="19.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="30.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="11.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="6.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="4.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="16.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="4.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="7.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="11.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="11.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="4.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="14.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="13.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="11.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="14.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="16.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="25" max="25" width="103.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="26" max="26" width="5.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="33.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="28" max="28" width="16.54296875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:28">
@@ -21363,20 +21355,20 @@
       <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="78.44140625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="13.21875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="4" width="11.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="23.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="11.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="13.21875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="11.77734375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="16.77734375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="11.77734375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="14.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="103.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="12.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="78.453125" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="13.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="4" width="11.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="23.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="11.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="13.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="11.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="16.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="11.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="14.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="103.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="12.1796875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14">
@@ -21701,20 +21693,20 @@
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="119.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="119.453125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="11" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="4" width="11.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="23.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="7" width="9.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="4" width="11.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="23.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="7" width="9.81640625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="8" max="8" width="17" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="11.77734375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="103.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="5.77734375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="10.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="11.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="103.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="5.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="10.1796875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="13" max="13" width="8" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="10.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="10.81640625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14">
@@ -21904,27 +21896,27 @@
   <sheetPr codeName="Sheet15"/>
   <dimension ref="A1:R4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="42.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="42.54296875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="11" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="4" width="11.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="20.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="18.21875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="9.77734375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="13.21875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="11.77734375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="11" width="16.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="4" width="11.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="20.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="18.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="9.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="13.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="11.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="11" width="16.81640625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="12" max="12" width="16" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="12.77734375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="13.21875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="11.77734375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="14.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="255.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="12.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="13.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="11.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="14.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="255.54296875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18">
@@ -22165,29 +22157,29 @@
       <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="79.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="79.453125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="11" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="4" width="17.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="4" width="17.1796875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="13" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="9.77734375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="15.21875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="9.77734375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="13.21875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="11.77734375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="16.77734375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="11.77734375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="14.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="103.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="5.77734375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="12.21875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="13.21875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="16.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="9.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="15.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="9.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="13.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="11.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="16.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="11.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="14.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="103.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="5.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="12.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="13.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="16.81640625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="19" max="19" width="16" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="20" max="20" width="13" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="12.77734375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="13.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="12.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="13.1796875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:22">
@@ -22336,29 +22328,29 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:W13"/>
   <sheetViews>
-    <sheetView topLeftCell="Q1" workbookViewId="0">
-      <selection activeCell="V17" sqref="V17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="160.77734375" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="36.5546875" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="31.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="11.77734375" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="160.81640625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="36.54296875" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="31.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="11.81640625" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="20" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="48.77734375" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="32.77734375" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="41.77734375" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="48.77734375" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="39.44140625" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="14.5546875" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="44.77734375" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="35.77734375" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="41.77734375" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="47.21875" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="188.21875" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="108.21875" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="48.81640625" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="32.81640625" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="41.81640625" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="48.81640625" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="39.453125" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="14.54296875" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="44.81640625" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="35.81640625" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="41.81640625" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="47.1796875" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="188.1796875" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="108.1796875" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:23">
@@ -22724,7 +22716,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="6" spans="1:23" ht="43.2">
+    <row r="6" spans="1:23" ht="43.5">
       <c r="A6" t="s">
         <v>80</v>
       </c>
@@ -22795,7 +22787,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="7" spans="1:23" ht="43.2">
+    <row r="7" spans="1:23" ht="43.5">
       <c r="A7" t="s">
         <v>87</v>
       </c>
@@ -22866,7 +22858,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="8" spans="1:23" ht="43.2">
+    <row r="8" spans="1:23" ht="43.5">
       <c r="A8" t="s">
         <v>88</v>
       </c>
@@ -22937,7 +22929,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="9" spans="1:23" ht="43.2">
+    <row r="9" spans="1:23" ht="43.5">
       <c r="A9" t="s">
         <v>89</v>
       </c>
@@ -23221,7 +23213,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="13" spans="1:23" ht="43.2">
+    <row r="13" spans="1:23" ht="43.5">
       <c r="A13" t="s">
         <v>96</v>
       </c>
@@ -23306,22 +23298,22 @@
       <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="79.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="79.54296875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="11" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="4" width="17.21875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="20.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="9.77734375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="17.21875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="13.21875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="16.77734375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="11.77734375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="14.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="103.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="5.77734375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="12.21875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="13.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="4" width="17.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="20.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="9.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="17.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="13.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="16.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="11.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="14.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="103.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="5.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="12.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="13.1796875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15">
@@ -23620,26 +23612,26 @@
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="95.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="95.81640625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="11" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="4" width="15.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="14.21875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="15.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="4" width="15.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="14.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="15.1796875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="7" max="7" width="10" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="31.77734375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="13.21875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="11.77734375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="16.77734375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="13.21875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="11.77734375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="14.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="22.77734375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="5.77734375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="9.21875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="11.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="16.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="31.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="13.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="11.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="16.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="13.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="11.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="14.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="22.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="5.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="9.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="11.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="16.81640625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19">
@@ -23834,17 +23826,17 @@
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="52.77734375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="3" width="16.21875" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="52.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="3" width="16.1796875" customWidth="1" collapsed="1"/>
     <col min="4" max="4" width="11" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="6" width="11.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="22.21875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="16.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="21.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="18.77734375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="16.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="6" width="11.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="22.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="16.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="21.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="18.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="16.81640625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
@@ -24176,22 +24168,22 @@
       <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="89.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="89.1796875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="11" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="4" width="11.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="22.21875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="10.21875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="23.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="20.77734375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="20.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="13.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="4" width="11.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="22.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="10.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="23.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="20.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="20.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="13.1796875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="11" max="11" width="17" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="11.77734375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="14.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="255.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="5.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="11.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="14.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="255.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="5.81640625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="16" max="16" width="10" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
@@ -26007,55 +25999,55 @@
   <dimension ref="A1:AQ70"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A65" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="E75" sqref="E75"/>
+      <selection pane="bottomLeft" activeCell="B70" sqref="B70"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="30.77734375" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="58.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="30.81640625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="58.81640625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="17" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="4" max="4" width="11" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="23" style="31" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="17.5546875" style="31" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="176.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="14.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="17.54296875" style="31" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="176.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="14.1796875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="9" max="9" width="16" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="11.77734375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="7.77734375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="6.5546875" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="5.21875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="7.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="5.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="22.77734375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="12.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="5.21875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="7.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="11.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="7.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="6.54296875" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="5.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="7.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="5.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="22.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="12.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="5.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="7.81640625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="20" max="20" width="8" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="11.21875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="14.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="11.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="14.1796875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="23" max="23" width="16" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="24" max="24" width="9" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="25" max="25" width="5.21875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="26" max="26" width="11.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="27" max="27" width="36.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="28" max="29" width="20.77734375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="30" max="30" width="14.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="31" max="31" width="16.77734375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="32" max="32" width="13.21875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="33" max="33" width="11.77734375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="34" max="34" width="14.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="35" max="35" width="20.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="36" max="36" width="14.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="37" max="37" width="39.21875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="38" max="38" width="9.21875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="39" max="39" width="21.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="25" max="25" width="5.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="26" max="26" width="11.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="36.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="28" max="29" width="20.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="30" max="30" width="14.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="31" max="31" width="16.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="32" max="32" width="13.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="33" max="33" width="11.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="34" max="34" width="14.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="35" max="35" width="20.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="36" max="36" width="14.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="37" max="37" width="39.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="38" max="38" width="9.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="39" max="39" width="21.54296875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="40" max="40" width="12" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="41" max="41" width="12.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="42" max="42" width="9.21875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="43" max="43" width="10.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="41" max="41" width="12.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="42" max="42" width="9.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="43" max="43" width="10.1796875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:43">
@@ -29202,7 +29194,7 @@
         <v>621</v>
       </c>
     </row>
-    <row r="25" spans="1:43" ht="14.1" customHeight="1">
+    <row r="25" spans="1:43" ht="14.15" customHeight="1">
       <c r="A25" t="s">
         <v>1151</v>
       </c>
@@ -35245,32 +35237,32 @@
       <selection activeCell="U32" sqref="U32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="79.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="12.77734375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="38.21875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="9.77734375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="38.21875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="21.77734375" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="17.21875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="41.77734375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="34.21875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="64.77734375" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="15.44140625" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="17.77734375" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="17.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="15" width="24.77734375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="25.21875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="14.21875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="17.21875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="7.21875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="23.77734375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="105.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="79.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="12.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="38.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="9.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="38.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="21.81640625" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="17.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="41.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="34.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="64.81640625" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="15.453125" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="17.81640625" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="17.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="15" width="24.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="25.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="14.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="17.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="7.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="23.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="105.453125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="22" max="22" width="17" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="16.21875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="24" max="24" width="43.77734375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="25" max="25" width="17.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="16.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="43.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="25" max="25" width="17.81640625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26">
@@ -35593,7 +35585,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:26" ht="13.05" customHeight="1">
+    <row r="5" spans="1:26" ht="13" customHeight="1">
       <c r="A5" s="13" t="s">
         <v>1432</v>
       </c>
@@ -38168,14 +38160,14 @@
       <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="24.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="11.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="18.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="22.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="24.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="11.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="18.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="22.54296875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="13" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="11.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="11.54296875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -38233,29 +38225,29 @@
       <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="81.21875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="3" width="16.21875" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="16.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="81.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="3" width="16.1796875" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="16.81640625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="11" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="6" max="6" width="11" customWidth="1"/>
-    <col min="7" max="8" width="11.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="8" width="11.453125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="9" max="9" width="13" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="16.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="18.77734375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="25.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="22.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="26.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="16" width="56.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="56.5546875" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="39.21875" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="28.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="38.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="25.21875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="42.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="29.21875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="24" max="24" width="10.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="16.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="18.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="25.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="22.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="26.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="16" width="56.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="56.54296875" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="39.1796875" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="28.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="38.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="25.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="42.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="29.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="10.1796875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26">
@@ -39472,29 +39464,29 @@
       <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="81.21875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="3" width="16.21875" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="16.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="81.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="3" width="16.1796875" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="16.81640625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="11" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="6" max="6" width="11" customWidth="1"/>
-    <col min="7" max="8" width="11.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="8" width="11.453125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="9" max="9" width="13" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="16.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="18.77734375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="25.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="22.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="26.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="16" width="56.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="56.5546875" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="39.21875" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="28.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="38.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="25.21875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="42.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="29.21875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="24" max="24" width="10.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="16.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="18.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="25.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="22.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="26.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="16" width="56.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="56.54296875" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="39.1796875" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="28.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="38.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="25.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="42.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="29.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="10.1796875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:27">
@@ -39676,29 +39668,29 @@
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="81.21875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="3" width="16.21875" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="16.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="81.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="3" width="16.1796875" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="16.81640625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="11" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="6" max="6" width="11" customWidth="1"/>
-    <col min="7" max="8" width="11.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="8" width="11.453125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="9" max="9" width="13" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="16.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="18.77734375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="25.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="22.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="26.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="16" width="56.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="56.5546875" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="39.21875" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="28.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="38.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="25.21875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="42.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="29.21875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="24" max="24" width="10.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="16.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="18.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="25.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="22.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="26.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="16" width="56.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="56.54296875" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="39.1796875" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="28.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="38.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="25.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="42.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="29.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="10.1796875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26">
@@ -40915,11 +40907,11 @@
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="18.21875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="30.77734375" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="14.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="18.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="30.81640625" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="14.81640625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -41089,34 +41081,34 @@
       <selection activeCell="AD7" sqref="AD7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="81.21875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="12.44140625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="14.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="81.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="12.453125" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="14.81640625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="4" max="4" width="11" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="34.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="33.77734375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="8" width="33.77734375" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="13.77734375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="28.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="24.77734375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="16" width="24.44140625" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="8.77734375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="15.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="70.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="25.77734375" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="25.5546875" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="77.21875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="23" max="24" width="25.77734375" customWidth="1" collapsed="1"/>
-    <col min="25" max="25" width="38.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="26" max="27" width="38.44140625" customWidth="1" collapsed="1"/>
-    <col min="28" max="28" width="39.21875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="29" max="30" width="39.21875" customWidth="1" collapsed="1"/>
-    <col min="31" max="31" width="43.21875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="32" max="33" width="43.21875" customWidth="1" collapsed="1"/>
-    <col min="34" max="34" width="27.77734375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="35" max="35" width="40.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="34.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="33.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="8" width="33.81640625" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="13.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="28.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="24.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="16" width="24.453125" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="8.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="15.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="70.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="25.81640625" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="25.54296875" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="77.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="23" max="24" width="25.81640625" customWidth="1" collapsed="1"/>
+    <col min="25" max="25" width="38.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="26" max="27" width="38.453125" customWidth="1" collapsed="1"/>
+    <col min="28" max="28" width="39.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="29" max="30" width="39.1796875" customWidth="1" collapsed="1"/>
+    <col min="31" max="31" width="43.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="32" max="33" width="43.1796875" customWidth="1" collapsed="1"/>
+    <col min="34" max="34" width="27.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="35" max="35" width="40.453125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:35">
@@ -43807,21 +43799,21 @@
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="145.21875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="10.77734375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="14.77734375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="16.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="145.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="10.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="14.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="16.81640625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="11" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="11.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="17.21875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="17.77734375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="17.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="11.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="17.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="17.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="17.54296875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="10" max="10" width="23" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="20.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="20.54296875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="12" max="12" width="27" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="9.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="9.81640625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13">
@@ -44001,13 +43993,13 @@
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="47" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="11.77734375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="17.21875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="14.77734375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="15.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="11.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="17.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="14.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="15.81640625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
@@ -44226,12 +44218,12 @@
       <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="53.44140625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="13.77734375" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="18.21875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="11.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="53.453125" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="13.81640625" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="18.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="11.81640625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -44443,15 +44435,15 @@
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="39.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="11.77734375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="14.21875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="14.77734375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="16.77734375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="17.21875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="18.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="39.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="11.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="14.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="14.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="16.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="17.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="18.1796875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
@@ -44573,13 +44565,13 @@
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="25.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="25.54296875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="2" max="3" width="11" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="14.77734375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="16.77734375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="11.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="14.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="16.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="11.81640625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -44635,20 +44627,20 @@
       <selection activeCell="B22" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="26.77734375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="88.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="26.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="88.453125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="17" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="11.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="11.81640625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="17" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="11.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="10" width="18.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="15.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="23.88671875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="31.21875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="15.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="75.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="11.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="10" width="18.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="15.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="23.90625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="31.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="15.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="75.54296875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17">
@@ -45353,20 +45345,20 @@
       <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="26.77734375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="88.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="26.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="88.453125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="17" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="11.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="11.81640625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="17" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="11.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="10" width="18.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="15.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="23.88671875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="31.21875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="15.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="75.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="11.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="10" width="18.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="15.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="23.90625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="31.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="15.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="75.54296875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17">
@@ -45541,17 +45533,17 @@
       <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="109.77734375" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="18.44140625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="39.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="109.81640625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="18.453125" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="39.1796875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="4" max="4" width="15" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="30.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="34.77734375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="18.21875" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="16.77734375" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="16.21875" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="30.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="34.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="18.1796875" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="16.81640625" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="16.1796875" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -45586,7 +45578,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="16.8">
+    <row r="2" spans="1:10" ht="16.5">
       <c r="A2" t="s">
         <v>1786</v>
       </c>
@@ -45728,21 +45720,21 @@
       <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="80.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="80.54296875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="11" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="16.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="16.77734375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="15.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="21.77734375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="14.77734375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="9.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="14.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="21.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="16.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="16.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="15.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="21.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="14.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="9.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="14.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="21.81640625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="15" max="15" width="16" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="14.21875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="14.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="14.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="14.81640625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18">
@@ -46263,72 +46255,72 @@
       <selection activeCell="BF8" sqref="BF8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="84.21875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="11.77734375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="17.77734375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="40.21875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="15.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="11.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="84.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="11.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="17.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="40.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="15.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="11.54296875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="7" max="7" width="13" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="15.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="12.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="15.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="12.453125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="10" max="10" width="12" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="17.21875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="51.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="17.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="51.453125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="13" max="13" width="15" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="10.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="11.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="3.77734375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="15.21875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="17.21875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="28.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="23.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="18.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="28.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="25.21875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="24" max="24" width="12.77734375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="25" max="25" width="3.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="10.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="11.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="3.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="15.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="17.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="28.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="23.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="18.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="28.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="25.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="12.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="25" max="25" width="3.81640625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="26" max="26" width="7" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="27" max="27" width="9.77734375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="28" max="28" width="17.77734375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="29" max="29" width="5.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="9.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="28" max="28" width="17.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="29" max="29" width="5.54296875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="30" max="30" width="10" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="31" max="31" width="12.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="32" max="32" width="11.77734375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="33" max="33" width="16.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="34" max="34" width="7.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="35" max="35" width="10.21875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="36" max="36" width="4.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="31" max="31" width="12.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="32" max="32" width="11.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="33" max="33" width="16.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="34" max="34" width="7.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="35" max="35" width="10.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="36" max="36" width="4.81640625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="37" max="37" width="9" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="38" max="38" width="6.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="39" max="39" width="11.77734375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="40" max="40" width="7.77734375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="41" max="41" width="11.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="42" max="42" width="13.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="38" max="38" width="6.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="39" max="39" width="11.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="40" max="40" width="7.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="41" max="41" width="11.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="42" max="42" width="13.453125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="43" max="43" width="14" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="44" max="44" width="13.21875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="45" max="45" width="7.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="46" max="46" width="13.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="44" max="44" width="13.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="45" max="45" width="7.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="46" max="46" width="13.1796875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="48" max="48" width="10" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="49" max="49" width="5.77734375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="50" max="50" width="6.77734375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="51" max="51" width="7.21875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="52" max="52" width="9.77734375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="53" max="53" width="10.77734375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="54" max="54" width="14.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="49" max="49" width="5.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="50" max="50" width="6.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="51" max="51" width="7.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="52" max="52" width="9.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="53" max="53" width="10.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="54" max="54" width="14.81640625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="55" max="55" width="20" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="56" max="56" width="8.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="57" max="57" width="8.77734375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="58" max="60" width="19.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="61" max="61" width="12.77734375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="62" max="62" width="10.21875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="63" max="63" width="24.77734375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="64" max="64" width="15.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="65" max="65" width="24.77734375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="66" max="66" width="16.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="67" max="67" width="5.77734375" customWidth="1" collapsed="1"/>
+    <col min="56" max="56" width="8.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="57" max="57" width="8.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="58" max="60" width="19.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="61" max="61" width="12.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="62" max="62" width="10.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="63" max="63" width="24.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="64" max="64" width="15.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="65" max="65" width="24.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="66" max="66" width="16.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="67" max="67" width="5.81640625" customWidth="1" collapsed="1"/>
     <col min="68" max="70" width="13" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
@@ -49327,15 +49319,15 @@
       <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="19.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="19.81640625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="11" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="11.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="17.21875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="7.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="14.77734375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="15.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="11.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="17.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="7.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="14.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="15.81640625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="8" max="8" width="17" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
@@ -49404,26 +49396,26 @@
       <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="77.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="77.54296875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="11" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="12.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="14.77734375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="20.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="12.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="14.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="20.54296875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="6" max="6" width="10" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="8" width="18.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="8" width="18.54296875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="9" max="9" width="18" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="10" max="10" width="19" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="21.77734375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="8.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="15.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="11.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="16.77734375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="20.77734375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="16.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="21.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="8.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="15.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="11.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="16.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="20.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="16.81640625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="18" max="18" width="16" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="13.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="13.1796875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19">
@@ -50090,14 +50082,14 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="74" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="11.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="11.453125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="11" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="4" max="4" width="13" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="9.77734375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="10.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="9.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="10.1796875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -50273,17 +50265,17 @@
       <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="113.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="113.1796875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="11" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="11.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="14.21875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="6" width="9.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="11.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="14.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="6" width="9.81640625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="7" max="7" width="17" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="11.77734375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="10" width="17.21875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="38.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="11.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="10" width="17.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="38.54296875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
@@ -50475,19 +50467,19 @@
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="83.77734375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="11.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="21.77734375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="29.21875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="21.21875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="25.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="15.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="83.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="11.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="21.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="29.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="21.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="25.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="15.54296875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="8" max="8" width="11" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="197.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="10.21875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="19.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="197.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="10.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="19.81640625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
@@ -50784,20 +50776,20 @@
       <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="85.21875" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="21.21875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="11.77734375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="24.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="16.77734375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="17.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="11.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="85.1796875" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="21.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="11.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="24.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="16.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="17.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="11.81640625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="8" max="8" width="11" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="33.77734375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="8.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="28.21875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="15.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="33.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="8.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="28.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="15.54296875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
@@ -51840,9 +51832,9 @@
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="57.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="57.54296875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -51878,20 +51870,20 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="67.21875" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="24.21875" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="24.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="18.21875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="24.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="19.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="67.1796875" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="24.1796875" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="24.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="18.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="24.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="19.1796875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="7" max="7" width="16" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="255.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="255.81640625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="10" max="10" width="18" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="11.77734375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="15.44140625" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="25.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="11.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="15.453125" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="25.81640625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16">
@@ -52508,9 +52500,9 @@
       <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="19.21875" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="19.1796875" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="79.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="79.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -52619,20 +52611,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2F00-000000000000}">
   <dimension ref="A1:AH9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="52.21875" customWidth="1"/>
-    <col min="6" max="6" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.5546875" customWidth="1"/>
+    <col min="1" max="1" width="41.36328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.36328125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.54296875" customWidth="1"/>
     <col min="17" max="17" width="13" customWidth="1"/>
-    <col min="27" max="27" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="31" max="33" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="31" max="33" width="12.6328125" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="19.6328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:34">
@@ -52730,7 +52721,7 @@
         <v>440</v>
       </c>
       <c r="AF1" s="11" t="s">
-        <v>1968</v>
+        <v>1969</v>
       </c>
       <c r="AG1" s="11" t="s">
         <v>441</v>
@@ -52834,7 +52825,7 @@
         <v>1958</v>
       </c>
       <c r="AF2" s="11" t="s">
-        <v>1969</v>
+        <v>1970</v>
       </c>
       <c r="AG2" s="11" t="s">
         <v>1958</v>
@@ -52938,7 +52929,7 @@
         <v>1958</v>
       </c>
       <c r="AF3" s="11" t="s">
-        <v>1969</v>
+        <v>1970</v>
       </c>
       <c r="AG3" s="11" t="s">
         <v>1958</v>
@@ -53042,7 +53033,7 @@
         <v>1958</v>
       </c>
       <c r="AF4" s="11" t="s">
-        <v>1969</v>
+        <v>1970</v>
       </c>
       <c r="AG4" s="11" t="s">
         <v>1958</v>
@@ -53146,7 +53137,7 @@
         <v>1958</v>
       </c>
       <c r="AF5" s="11" t="s">
-        <v>1969</v>
+        <v>1970</v>
       </c>
       <c r="AG5" s="11" t="s">
         <v>1958</v>
@@ -53157,7 +53148,7 @@
     </row>
     <row r="6" spans="1:34">
       <c r="A6" s="91" t="s">
-        <v>1967</v>
+        <v>1968</v>
       </c>
       <c r="B6" s="92" t="s">
         <v>106</v>
@@ -53250,7 +53241,7 @@
         <v>1966</v>
       </c>
       <c r="AF6" s="11" t="s">
-        <v>1969</v>
+        <v>1970</v>
       </c>
       <c r="AG6" s="11" t="s">
         <v>1966</v>
@@ -53261,7 +53252,7 @@
     </row>
     <row r="7" spans="1:34">
       <c r="A7" s="91" t="s">
-        <v>1970</v>
+        <v>1967</v>
       </c>
       <c r="B7" s="92" t="s">
         <v>106</v>
@@ -53279,7 +53270,7 @@
         <v>82</v>
       </c>
       <c r="G7" s="94" t="s">
-        <v>1973</v>
+        <v>1950</v>
       </c>
       <c r="H7" s="95" t="s">
         <v>24</v>
@@ -53345,7 +53336,7 @@
         <v>752</v>
       </c>
       <c r="AC7" s="93" t="s">
-        <v>17</v>
+        <v>1752</v>
       </c>
       <c r="AD7" s="93" t="s">
         <v>1752</v>
@@ -53354,7 +53345,7 @@
         <v>1958</v>
       </c>
       <c r="AF7" s="11" t="s">
-        <v>1969</v>
+        <v>1970</v>
       </c>
       <c r="AG7" s="11" t="s">
         <v>1958</v>
@@ -53364,8 +53355,8 @@
       </c>
     </row>
     <row r="8" spans="1:34">
-      <c r="A8" s="91" t="s">
-        <v>1972</v>
+      <c r="A8" s="96" t="s">
+        <v>1971</v>
       </c>
       <c r="B8" s="92" t="s">
         <v>106</v>
@@ -53383,7 +53374,7 @@
         <v>82</v>
       </c>
       <c r="G8" s="94" t="s">
-        <v>1971</v>
+        <v>1950</v>
       </c>
       <c r="H8" s="95" t="s">
         <v>24</v>
@@ -53443,7 +53434,7 @@
         <v>26</v>
       </c>
       <c r="AA8" s="93" t="s">
-        <v>1944</v>
+        <v>1946</v>
       </c>
       <c r="AB8" s="93" t="s">
         <v>1944</v>
@@ -53455,21 +53446,21 @@
         <v>1752</v>
       </c>
       <c r="AE8" s="11" t="s">
-        <v>1958</v>
+        <v>224</v>
       </c>
       <c r="AF8" s="11" t="s">
-        <v>1969</v>
+        <v>1970</v>
       </c>
       <c r="AG8" s="11" t="s">
-        <v>1958</v>
+        <v>224</v>
       </c>
       <c r="AH8" s="11" t="s">
         <v>1959</v>
       </c>
     </row>
     <row r="9" spans="1:34">
-      <c r="A9" s="91" t="s">
-        <v>1975</v>
+      <c r="A9" s="96" t="s">
+        <v>1972</v>
       </c>
       <c r="B9" s="92" t="s">
         <v>106</v>
@@ -53547,32 +53538,31 @@
         <v>26</v>
       </c>
       <c r="AA9" s="93" t="s">
+        <v>477</v>
+      </c>
+      <c r="AB9" s="93" t="s">
         <v>1946</v>
       </c>
-      <c r="AB9" s="93" t="s">
-        <v>1944</v>
-      </c>
       <c r="AC9" s="93" t="s">
-        <v>1752</v>
+        <v>1973</v>
       </c>
       <c r="AD9" s="93" t="s">
-        <v>1752</v>
+        <v>1973</v>
       </c>
       <c r="AE9" s="11" t="s">
-        <v>1976</v>
+        <v>224</v>
       </c>
       <c r="AF9" s="11" t="s">
-        <v>1969</v>
+        <v>1970</v>
       </c>
       <c r="AG9" s="11" t="s">
-        <v>1976</v>
+        <v>224</v>
       </c>
       <c r="AH9" s="11" t="s">
-        <v>1977</v>
+        <v>1959</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -53582,79 +53572,79 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:BW35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A11" workbookViewId="0">
       <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="78.44140625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="11.77734375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="17.77734375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="25.21875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="15.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="11.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="78.453125" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="11.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="17.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="25.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="15.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="11.54296875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="7" max="7" width="13" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="15.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="12.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="15.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="12.453125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="10" max="10" width="12" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="17.21875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="15" width="17.21875" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="17.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="15" width="17.1796875" customWidth="1" collapsed="1"/>
     <col min="16" max="16" width="25" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="17.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="17.1796875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="18" max="19" width="15" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="10.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="11.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="4.77734375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="15.21875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="24" max="24" width="17.21875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="25" max="25" width="28.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="26" max="26" width="23.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="27" max="27" width="18.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="28" max="28" width="28.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="29" max="29" width="25.21875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="30" max="30" width="12.77734375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="31" max="31" width="3.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="10.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="11.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="4.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="15.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="17.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="25" max="25" width="28.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="26" max="26" width="23.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="18.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="28" max="28" width="28.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="29" max="29" width="25.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="30" max="30" width="12.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="31" max="31" width="3.81640625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="32" max="32" width="7" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="33" max="33" width="9.77734375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="34" max="34" width="17.77734375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="35" max="35" width="5.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="33" max="33" width="9.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="34" max="34" width="17.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="35" max="35" width="5.54296875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="36" max="36" width="10" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="37" max="37" width="12.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="38" max="38" width="11.77734375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="39" max="39" width="16.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="40" max="40" width="7.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="41" max="41" width="10.21875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="42" max="42" width="4.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="37" max="37" width="12.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="38" max="38" width="11.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="39" max="39" width="16.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="40" max="40" width="7.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="41" max="41" width="10.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="42" max="42" width="4.81640625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="43" max="43" width="9" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="44" max="44" width="6.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="45" max="45" width="11.77734375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="46" max="46" width="7.77734375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="47" max="47" width="11.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="48" max="48" width="13.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="44" max="44" width="6.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="45" max="45" width="11.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="46" max="46" width="7.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="47" max="47" width="11.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="48" max="48" width="13.453125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="49" max="49" width="14" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="50" max="50" width="13.21875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="51" max="51" width="7.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="52" max="52" width="13.21875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="53" max="53" width="9.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="50" max="50" width="13.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="51" max="51" width="7.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="52" max="52" width="13.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="53" max="53" width="9.1796875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="54" max="54" width="10" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="55" max="55" width="5.77734375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="56" max="56" width="6.77734375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="57" max="57" width="7.21875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="58" max="58" width="9.77734375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="59" max="59" width="10.77734375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="60" max="60" width="12.77734375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="61" max="61" width="27.77734375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="62" max="63" width="11.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="64" max="66" width="19.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="67" max="67" width="12.77734375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="68" max="68" width="10.21875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="69" max="69" width="22.21875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="70" max="70" width="13.21875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="71" max="71" width="15.77734375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="72" max="73" width="24.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="55" max="55" width="5.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="56" max="56" width="6.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="57" max="57" width="7.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="58" max="58" width="9.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="59" max="59" width="10.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="60" max="60" width="12.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="61" max="61" width="27.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="62" max="63" width="11.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="64" max="66" width="19.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="67" max="67" width="12.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="68" max="68" width="10.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="69" max="69" width="22.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="70" max="70" width="13.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="71" max="71" width="15.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="72" max="73" width="24.81640625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="74" max="74" width="14" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="75" max="75" width="14.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="75" max="75" width="14.1796875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:71">
@@ -54129,7 +54119,7 @@
       </c>
       <c r="N3" t="str">
         <f t="shared" ref="N3:N4" ca="1" si="0">CONCATENATE(E3," ",TEXT(TODAY(),"mm-dd-yyyy"))</f>
-        <v>SICA 09-16-2025</v>
+        <v>SICA 09-15-2025</v>
       </c>
       <c r="O3" t="s">
         <v>202</v>
@@ -54345,7 +54335,7 @@
       </c>
       <c r="N4" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>MICA 09-16-2025</v>
+        <v>MICA 09-15-2025</v>
       </c>
       <c r="O4" t="s">
         <v>202</v>
@@ -61230,7 +61220,7 @@
       <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
@@ -61255,15 +61245,15 @@
       <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="51.21875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="5" width="15.5546875" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="16.77734375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="14.77734375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="13.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="25.21875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="25.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="51.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="5" width="15.54296875" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="16.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="14.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="13.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="25.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="25.453125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="16" max="16" width="22" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
@@ -61381,43 +61371,43 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="64" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="17.21875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="13.21875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="14.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="16.5546875" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="43.77734375" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="16.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="6.21875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="11.77734375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="5.77734375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="11.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="17.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="13.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="14.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="16.54296875" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="43.81640625" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="16.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="6.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="11.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="5.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="11.81640625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="13" max="13" width="17" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="14" max="14" width="11" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="13.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="17" width="11.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="13.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="17" width="11.453125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="18" max="18" width="15" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="13.21875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="11.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="21" max="23" width="13.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="25" max="25" width="11.21875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="26" max="26" width="57.21875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="27" max="27" width="19.77734375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="28" max="28" width="18.21875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="29" max="29" width="25.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="30" max="30" width="9.77734375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="31" max="31" width="11.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="32" max="32" width="36.21875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="33" max="33" width="31.21875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="34" max="34" width="16.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="13.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="11.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="23" width="13.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="25" max="25" width="11.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="26" max="26" width="57.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="19.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="28" max="28" width="18.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="29" max="29" width="25.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="30" max="30" width="9.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="31" max="31" width="11.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="32" max="32" width="36.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="33" max="33" width="31.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="34" max="34" width="16.81640625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="35" max="35" width="14" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="36" max="36" width="14.77734375" customWidth="1" collapsed="1"/>
-    <col min="37" max="37" width="15.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="38" max="38" width="11.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="36" max="36" width="14.81640625" customWidth="1" collapsed="1"/>
+    <col min="37" max="37" width="15.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="38" max="38" width="11.54296875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="39" max="39" width="13" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="40" max="40" width="11.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="40" max="40" width="11.54296875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="41" max="41" width="13" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
@@ -62935,49 +62925,49 @@
       <selection activeCell="AN10" sqref="AN10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="35.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.77734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.21875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.21875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.77734375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.77734375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.77734375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="6.77734375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.77734375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="6.5546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.77734375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.5546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="18.21875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="11.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="35.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.1796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.81640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.81640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.81640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.81640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.81640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="6.54296875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.54296875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="18.1796875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.81640625" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="13" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="25.44140625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="16.21875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="14.21875" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="11.21875" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="10.21875" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="11.21875" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="25.453125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="16.1796875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="14.1796875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="11.1796875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="10.1796875" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="11.1796875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="14.453125" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="11" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="9.21875" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="18.5546875" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="20.77734375" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="19.44140625" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="27.21875" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="12.21875" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="38.5546875" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="33.5546875" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="22.21875" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="9.1796875" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="18.54296875" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="20.81640625" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="19.453125" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="27.1796875" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="12.1796875" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="38.54296875" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="33.54296875" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="22.1796875" bestFit="1" customWidth="1"/>
     <col min="35" max="35" width="15" bestFit="1" customWidth="1"/>
     <col min="36" max="36" width="16" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="16.77734375" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="12.5546875" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="12.77734375" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="22.21875" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="17.21875" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="16.81640625" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="12.54296875" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="12.81640625" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="22.1796875" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="17.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:41">
@@ -63361,6 +63351,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="0af65dbd-c349-4f95-a569-a37e7dcda261">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="a705add3-b55d-4a21-9da5-61558d9a88d9" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101004775ACE7CF61FD429C250F0EADD242CB" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="bdc0ef193019ef7ec3c6044774d719fd">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="0af65dbd-c349-4f95-a569-a37e7dcda261" xmlns:ns3="a705add3-b55d-4a21-9da5-61558d9a88d9" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="5eb62fd137b9132ea1ed680202856fff" ns2:_="" ns3:_="">
     <xsd:import namespace="0af65dbd-c349-4f95-a569-a37e7dcda261"/>
@@ -63615,27 +63625,26 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C7BF3F34-769C-4AFA-8719-29B8EDC91EB1}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="0af65dbd-c349-4f95-a569-a37e7dcda261">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="a705add3-b55d-4a21-9da5-61558d9a88d9" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4B56E0B5-42C8-48C9-A658-2E92FF4B9C74}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="0af65dbd-c349-4f95-a569-a37e7dcda261"/>
+    <ds:schemaRef ds:uri="a705add3-b55d-4a21-9da5-61558d9a88d9"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F2911B9E-6765-44F9-94CA-04166374824D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -63652,23 +63661,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C7BF3F34-769C-4AFA-8719-29B8EDC91EB1}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4B56E0B5-42C8-48C9-A658-2E92FF4B9C74}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="0af65dbd-c349-4f95-a569-a37e7dcda261"/>
-    <ds:schemaRef ds:uri="a705add3-b55d-4a21-9da5-61558d9a88d9"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Added updates for JagadeeshCode branch
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/Test.xlsx
+++ b/src/test/resources/excel/Test.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rajeena.RR\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jagadeesh.Reddy\Desktop\ipim\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABA6644E-A84F-41D3-A7FF-C94092F99767}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2AFAAE7-1099-44EA-862C-39736FE85BC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="780" firstSheet="43" activeTab="48" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" tabRatio="780" firstSheet="45" activeTab="48" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AddCatalogs" sheetId="80" r:id="rId1"/>
@@ -87,7 +87,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17822" uniqueCount="1975">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17822" uniqueCount="1978">
   <si>
     <t>TestCaseName</t>
   </si>
@@ -5990,9 +5990,6 @@
     <t>GTIN</t>
   </si>
   <si>
-    <t>verify_Dimensions_iPIM_JSON_Verification_US</t>
-  </si>
-  <si>
     <t>verify_GTINAndClassCodesID_In_IPIMJson_US</t>
   </si>
   <si>
@@ -6002,16 +5999,28 @@
     <t>Pricing UOM</t>
   </si>
   <si>
-    <t>verify_Product_Description_JSON_Verification_US</t>
-  </si>
-  <si>
-    <t>verify_Product_Media_JSON_Verification_US</t>
-  </si>
-  <si>
-    <t>Media</t>
-  </si>
-  <si>
-    <t>5803732</t>
+    <t>verify_Dimensions_ItemCategoryID_GlobalMessageID_NonBaseCatalogToProductMapping_ItemClassification_iPIM_JSON_Verification_US</t>
+  </si>
+  <si>
+    <t>6037773</t>
+  </si>
+  <si>
+    <t>verify_Prices_JSON_Verification_US</t>
+  </si>
+  <si>
+    <t>5803430</t>
+  </si>
+  <si>
+    <t>9870464</t>
+  </si>
+  <si>
+    <t>verify_Competitor_Price_JSON_Verification_US</t>
+  </si>
+  <si>
+    <t>Alternative item no. (selling, &lt;Public&gt;)</t>
+  </si>
+  <si>
+    <t>Competitor_ACESOUTH</t>
   </si>
 </sst>
 </file>
@@ -6238,7 +6247,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="97">
+  <cellXfs count="96">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
@@ -6369,7 +6378,6 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -6668,26 +6676,26 @@
       <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="46.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="21.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="46.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="21.77734375" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="11" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="5" width="15.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="23.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="10.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="11.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="22.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="20.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="15.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="17.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="16.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="18.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="14.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="15.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="18" width="18.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="12.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="22.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="5" width="15.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="23.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="10.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="11.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="22.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="20.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="15.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="17.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="16.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="18.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="14.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="15.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="18" width="18.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="12.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="22.21875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20">
@@ -7075,21 +7083,21 @@
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="149.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="149.5546875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="11" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="17" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="17.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="6" width="11.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="17.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="14.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="20.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="27.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="255.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="5.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="11.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="21.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="17.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="6" width="11.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="17.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="14.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="20.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="27.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="255.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="5.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="11.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="21.44140625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14">
@@ -7193,47 +7201,47 @@
       <selection activeCell="S1" sqref="S1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="96" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="16.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="16.81640625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="16.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="16.77734375" customWidth="1" collapsed="1"/>
     <col min="4" max="4" width="11" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="6" width="11.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="21.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="10" width="21.1796875" customWidth="1" collapsed="1"/>
+    <col min="5" max="6" width="11.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="21.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="10" width="21.21875" customWidth="1" collapsed="1"/>
     <col min="11" max="11" width="13" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="16.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="16.453125" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="18.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="25.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="25.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="22.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="39.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="22" width="39.1796875" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="28.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="24" max="24" width="25.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="25" max="25" width="29.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="26" max="26" width="29.1796875" customWidth="1" collapsed="1"/>
-    <col min="27" max="27" width="10.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="16.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="16.44140625" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="18.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="25.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="25.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="22.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="39.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="22" width="39.21875" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="28.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="25.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="25" max="25" width="29.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="26" max="26" width="29.21875" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="10.21875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="28" max="28" width="108" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="29" max="29" width="25.54296875" customWidth="1" collapsed="1"/>
-    <col min="30" max="30" width="49.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="31" max="31" width="35.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="32" max="32" width="35.54296875" customWidth="1" collapsed="1"/>
-    <col min="33" max="33" width="132.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="34" max="35" width="27.453125" customWidth="1" collapsed="1"/>
+    <col min="29" max="29" width="25.5546875" customWidth="1" collapsed="1"/>
+    <col min="30" max="30" width="49.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="31" max="31" width="35.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="32" max="32" width="35.5546875" customWidth="1" collapsed="1"/>
+    <col min="33" max="33" width="132.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="34" max="35" width="27.44140625" customWidth="1" collapsed="1"/>
     <col min="36" max="36" width="32" customWidth="1" collapsed="1"/>
-    <col min="37" max="37" width="46.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="38" max="39" width="25.81640625" customWidth="1" collapsed="1"/>
-    <col min="40" max="40" width="32.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="41" max="41" width="47.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="42" max="43" width="35.81640625" customWidth="1" collapsed="1"/>
-    <col min="44" max="44" width="32.81640625" customWidth="1" collapsed="1"/>
-    <col min="45" max="45" width="51.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="46" max="47" width="33.453125" customWidth="1" collapsed="1"/>
-    <col min="48" max="49" width="32.81640625" customWidth="1" collapsed="1"/>
-    <col min="50" max="50" width="38.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="37" max="37" width="46.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="38" max="39" width="25.77734375" customWidth="1" collapsed="1"/>
+    <col min="40" max="40" width="32.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="41" max="41" width="47.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="42" max="43" width="35.77734375" customWidth="1" collapsed="1"/>
+    <col min="44" max="44" width="32.77734375" customWidth="1" collapsed="1"/>
+    <col min="45" max="45" width="51.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="46" max="47" width="33.44140625" customWidth="1" collapsed="1"/>
+    <col min="48" max="49" width="32.77734375" customWidth="1" collapsed="1"/>
+    <col min="50" max="50" width="38.21875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:50">
@@ -7996,7 +8004,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="1:50" ht="15.65" customHeight="1">
+    <row r="6" spans="1:50" ht="15.6" customHeight="1">
       <c r="A6" t="s">
         <v>488</v>
       </c>
@@ -12722,23 +12730,23 @@
       <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="48.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="48.21875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="11" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="21.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="13.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="8.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="7" width="12.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="8.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="14.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="11.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="7.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="8.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="11.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="9.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="21.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="17" width="11.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="21.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="13.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="8.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="7" width="12.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="8.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="14.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="11.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="7.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="8.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="11.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="9.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="21.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="17" width="11.44140625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17">
@@ -13333,31 +13341,31 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:T62"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:XFD2"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="87.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="87.44140625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="11" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="4" width="11.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="23.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="11.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="9.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="13.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="18.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="4" width="11.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="23.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="11.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="9.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="13.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="18.77734375" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="10" max="10" width="17" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="11.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="14.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="255.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="5.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="10.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="36.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="12.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="13.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="13.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="11.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="14.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="255.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="5.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="10.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="36.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="12.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="13.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="13.77734375" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="20" max="20" width="19" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
@@ -17220,28 +17228,28 @@
       <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="128.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="128.21875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="11" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="4" width="11.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="13.54296875" customWidth="1" collapsed="1"/>
+    <col min="3" max="4" width="11.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="13.5546875" customWidth="1" collapsed="1"/>
     <col min="6" max="6" width="13" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="20.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="9.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="35.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="13.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="11.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="16.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="11.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="14.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="103.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="5.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="193.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="16.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="12.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="14.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="11.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="20.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="9.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="35.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="13.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="11.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="16.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="11.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="14.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="103.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="5.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="193.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="16.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="12.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="14.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="11.5546875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21">
@@ -18040,35 +18048,35 @@
       <selection activeCell="A43" sqref="A43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="84.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="3" width="11.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="16.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="84.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="3" width="11.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="16.77734375" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="11" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="20.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="64.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="16.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="19.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="30.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="11.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="6.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="4.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="16.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="4.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="7.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="11.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="11.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="4.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="14.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="13.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="11.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="14.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="24" max="24" width="16.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="25" max="25" width="103.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="26" max="26" width="5.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="27" max="27" width="33.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="28" max="28" width="16.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="20.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="64.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="16.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="19.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="30.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="11.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="6.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="4.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="16.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="4.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="7.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="11.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="11.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="4.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="14.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="13.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="11.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="14.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="16.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="25" max="25" width="103.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="26" max="26" width="5.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="33.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="28" max="28" width="16.5546875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:28">
@@ -21355,20 +21363,20 @@
       <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="78.453125" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="13.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="4" width="11.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="23.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="11.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="13.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="11.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="16.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="11.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="14.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="103.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="12.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="78.44140625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="13.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="4" width="11.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="23.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="11.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="13.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="11.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="16.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="11.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="14.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="103.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="12.21875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14">
@@ -21693,20 +21701,20 @@
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="119.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="119.44140625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="11" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="4" width="11.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="23.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="7" width="9.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="4" width="11.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="23.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="7" width="9.77734375" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="8" max="8" width="17" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="11.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="103.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="5.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="10.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="11.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="103.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="5.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="10.21875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="13" max="13" width="8" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="10.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="10.77734375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14">
@@ -21896,27 +21904,27 @@
   <sheetPr codeName="Sheet15"/>
   <dimension ref="A1:R4"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="42.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="42.5546875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="11" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="4" width="11.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="20.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="18.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="9.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="13.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="11.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="11" width="16.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="4" width="11.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="20.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="18.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="9.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="13.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="11.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="11" width="16.77734375" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="12" max="12" width="16" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="12.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="13.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="11.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="14.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="255.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="12.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="13.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="11.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="14.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="255.5546875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18">
@@ -22157,29 +22165,29 @@
       <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="79.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="79.44140625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="11" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="4" width="17.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="4" width="17.21875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="13" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="9.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="15.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="9.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="13.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="11.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="16.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="11.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="14.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="103.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="5.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="12.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="13.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="16.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="9.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="15.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="9.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="13.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="11.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="16.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="11.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="14.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="103.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="5.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="12.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="13.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="16.77734375" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="19" max="19" width="16" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="20" max="20" width="13" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="12.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="13.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="12.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="13.21875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:22">
@@ -22328,29 +22336,29 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:W13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView topLeftCell="Q1" workbookViewId="0">
+      <selection activeCell="V17" sqref="V17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="160.81640625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="36.54296875" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="31.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="11.81640625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="160.77734375" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="36.5546875" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="31.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="11.77734375" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="20" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="48.81640625" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="32.81640625" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="41.81640625" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="48.81640625" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="39.453125" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="14.54296875" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="44.81640625" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="35.81640625" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="41.81640625" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="47.1796875" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="188.1796875" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="108.1796875" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="48.77734375" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="32.77734375" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="41.77734375" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="48.77734375" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="39.44140625" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="14.5546875" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="44.77734375" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="35.77734375" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="41.77734375" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="47.21875" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="188.21875" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="108.21875" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:23">
@@ -22716,7 +22724,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="6" spans="1:23" ht="43.5">
+    <row r="6" spans="1:23" ht="43.2">
       <c r="A6" t="s">
         <v>80</v>
       </c>
@@ -22787,7 +22795,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="7" spans="1:23" ht="43.5">
+    <row r="7" spans="1:23" ht="43.2">
       <c r="A7" t="s">
         <v>87</v>
       </c>
@@ -22858,7 +22866,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="8" spans="1:23" ht="43.5">
+    <row r="8" spans="1:23" ht="43.2">
       <c r="A8" t="s">
         <v>88</v>
       </c>
@@ -22929,7 +22937,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="9" spans="1:23" ht="43.5">
+    <row r="9" spans="1:23" ht="43.2">
       <c r="A9" t="s">
         <v>89</v>
       </c>
@@ -23213,7 +23221,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="13" spans="1:23" ht="43.5">
+    <row r="13" spans="1:23" ht="43.2">
       <c r="A13" t="s">
         <v>96</v>
       </c>
@@ -23298,22 +23306,22 @@
       <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="79.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="79.5546875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="11" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="4" width="17.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="20.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="9.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="17.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="13.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="16.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="11.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="14.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="103.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="5.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="12.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="13.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="4" width="17.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="20.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="9.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="17.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="13.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="16.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="11.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="14.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="103.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="5.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="12.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="13.21875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15">
@@ -23612,26 +23620,26 @@
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="95.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="95.77734375" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="11" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="4" width="15.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="14.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="15.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="4" width="15.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="14.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="15.21875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="7" max="7" width="10" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="31.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="13.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="11.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="16.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="13.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="11.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="14.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="22.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="5.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="9.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="11.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="16.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="31.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="13.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="11.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="16.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="13.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="11.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="14.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="22.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="5.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="9.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="11.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="16.77734375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19">
@@ -23826,17 +23834,17 @@
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="52.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="3" width="16.1796875" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="52.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="3" width="16.21875" customWidth="1" collapsed="1"/>
     <col min="4" max="4" width="11" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="6" width="11.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="22.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="16.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="21.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="18.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="16.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="6" width="11.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="22.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="16.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="21.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="18.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="16.77734375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
@@ -24168,22 +24176,22 @@
       <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="89.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="89.21875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="11" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="4" width="11.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="22.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="10.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="23.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="20.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="20.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="13.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="4" width="11.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="22.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="10.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="23.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="20.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="20.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="13.21875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="11" max="11" width="17" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="11.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="14.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="255.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="5.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="11.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="14.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="255.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="5.77734375" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="16" max="16" width="10" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
@@ -25999,55 +26007,55 @@
   <dimension ref="A1:AQ70"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A65" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="B70" sqref="B70"/>
+      <selection pane="bottomLeft" activeCell="E75" sqref="E75"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="30.81640625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="58.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="30.77734375" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="58.77734375" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="17" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="4" max="4" width="11" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="23" style="31" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="17.54296875" style="31" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="176.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="14.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="17.5546875" style="31" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="176.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="14.21875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="9" max="9" width="16" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="11.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="7.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="6.54296875" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="5.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="7.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="5.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="22.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="12.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="5.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="7.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="11.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="7.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="6.5546875" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="5.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="7.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="5.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="22.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="12.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="5.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="7.77734375" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="20" max="20" width="8" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="11.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="14.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="11.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="14.21875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="23" max="23" width="16" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="24" max="24" width="9" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="25" max="25" width="5.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="26" max="26" width="11.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="27" max="27" width="36.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="28" max="29" width="20.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="30" max="30" width="14.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="31" max="31" width="16.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="32" max="32" width="13.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="33" max="33" width="11.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="34" max="34" width="14.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="35" max="35" width="20.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="36" max="36" width="14.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="37" max="37" width="39.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="38" max="38" width="9.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="39" max="39" width="21.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="25" max="25" width="5.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="26" max="26" width="11.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="36.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="28" max="29" width="20.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="30" max="30" width="14.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="31" max="31" width="16.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="32" max="32" width="13.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="33" max="33" width="11.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="34" max="34" width="14.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="35" max="35" width="20.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="36" max="36" width="14.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="37" max="37" width="39.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="38" max="38" width="9.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="39" max="39" width="21.5546875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="40" max="40" width="12" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="41" max="41" width="12.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="42" max="42" width="9.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="43" max="43" width="10.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="41" max="41" width="12.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="42" max="42" width="9.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="43" max="43" width="10.21875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:43">
@@ -29194,7 +29202,7 @@
         <v>621</v>
       </c>
     </row>
-    <row r="25" spans="1:43" ht="14.15" customHeight="1">
+    <row r="25" spans="1:43" ht="14.1" customHeight="1">
       <c r="A25" t="s">
         <v>1151</v>
       </c>
@@ -35237,32 +35245,32 @@
       <selection activeCell="U32" sqref="U32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="79.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="12.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="38.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="9.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="38.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="21.81640625" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="17.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="41.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="34.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="64.81640625" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="15.453125" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="17.81640625" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="17.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="15" width="24.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="25.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="14.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="17.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="7.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="23.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="105.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="79.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="12.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="38.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="9.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="38.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="21.77734375" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="17.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="41.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="34.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="64.77734375" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="15.44140625" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="17.77734375" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="17.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="15" width="24.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="25.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="14.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="17.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="7.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="23.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="105.44140625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="22" max="22" width="17" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="16.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="24" max="24" width="43.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="25" max="25" width="17.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="16.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="43.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="25" max="25" width="17.77734375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26">
@@ -35585,7 +35593,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:26" ht="13" customHeight="1">
+    <row r="5" spans="1:26" ht="13.05" customHeight="1">
       <c r="A5" s="13" t="s">
         <v>1432</v>
       </c>
@@ -38160,14 +38168,14 @@
       <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="24.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="11.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="18.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="22.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="24.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="11.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="18.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="22.5546875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="13" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="11.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="11.5546875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -38225,29 +38233,29 @@
       <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="81.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="3" width="16.1796875" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="16.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="81.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="3" width="16.21875" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="16.77734375" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="11" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="6" max="6" width="11" customWidth="1"/>
-    <col min="7" max="8" width="11.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="8" width="11.44140625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="9" max="9" width="13" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="16.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="18.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="25.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="22.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="26.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="16" width="56.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="56.54296875" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="39.1796875" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="28.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="38.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="25.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="42.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="29.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="24" max="24" width="10.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="16.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="18.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="25.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="22.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="26.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="16" width="56.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="56.5546875" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="39.21875" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="28.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="38.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="25.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="42.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="29.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="10.21875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26">
@@ -39464,29 +39472,29 @@
       <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="81.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="3" width="16.1796875" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="16.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="81.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="3" width="16.21875" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="16.77734375" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="11" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="6" max="6" width="11" customWidth="1"/>
-    <col min="7" max="8" width="11.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="8" width="11.44140625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="9" max="9" width="13" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="16.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="18.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="25.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="22.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="26.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="16" width="56.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="56.54296875" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="39.1796875" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="28.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="38.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="25.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="42.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="29.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="24" max="24" width="10.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="16.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="18.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="25.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="22.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="26.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="16" width="56.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="56.5546875" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="39.21875" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="28.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="38.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="25.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="42.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="29.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="10.21875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:27">
@@ -39668,29 +39676,29 @@
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="81.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="3" width="16.1796875" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="16.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="81.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="3" width="16.21875" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="16.77734375" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="11" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="6" max="6" width="11" customWidth="1"/>
-    <col min="7" max="8" width="11.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="8" width="11.44140625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="9" max="9" width="13" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="16.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="18.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="25.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="22.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="26.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="16" width="56.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="56.54296875" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="39.1796875" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="28.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="38.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="25.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="42.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="29.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="24" max="24" width="10.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="16.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="18.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="25.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="22.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="26.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="16" width="56.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="56.5546875" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="39.21875" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="28.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="38.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="25.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="42.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="29.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="10.21875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26">
@@ -40907,11 +40915,11 @@
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="18.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="30.81640625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="14.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="18.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="30.77734375" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="14.77734375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -41081,34 +41089,34 @@
       <selection activeCell="AD7" sqref="AD7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="81.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="12.453125" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="14.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="81.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="12.44140625" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="14.77734375" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="4" max="4" width="11" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="34.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="33.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="8" width="33.81640625" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="13.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="28.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="24.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="16" width="24.453125" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="8.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="15.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="70.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="25.81640625" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="25.54296875" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="77.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="23" max="24" width="25.81640625" customWidth="1" collapsed="1"/>
-    <col min="25" max="25" width="38.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="26" max="27" width="38.453125" customWidth="1" collapsed="1"/>
-    <col min="28" max="28" width="39.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="29" max="30" width="39.1796875" customWidth="1" collapsed="1"/>
-    <col min="31" max="31" width="43.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="32" max="33" width="43.1796875" customWidth="1" collapsed="1"/>
-    <col min="34" max="34" width="27.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="35" max="35" width="40.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="34.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="33.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="8" width="33.77734375" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="13.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="28.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="24.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="16" width="24.44140625" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="8.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="15.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="70.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="25.77734375" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="25.5546875" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="77.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="23" max="24" width="25.77734375" customWidth="1" collapsed="1"/>
+    <col min="25" max="25" width="38.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="26" max="27" width="38.44140625" customWidth="1" collapsed="1"/>
+    <col min="28" max="28" width="39.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="29" max="30" width="39.21875" customWidth="1" collapsed="1"/>
+    <col min="31" max="31" width="43.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="32" max="33" width="43.21875" customWidth="1" collapsed="1"/>
+    <col min="34" max="34" width="27.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="35" max="35" width="40.44140625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:35">
@@ -43799,21 +43807,21 @@
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="145.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="10.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="14.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="16.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="145.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="10.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="14.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="16.77734375" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="11" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="11.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="17.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="17.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="17.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="11.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="17.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="17.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="17.5546875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="10" max="10" width="23" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="20.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="20.5546875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="12" max="12" width="27" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="9.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="9.77734375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13">
@@ -43993,13 +44001,13 @@
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="47" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="11.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="17.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="14.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="15.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="11.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="17.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="14.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="15.77734375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
@@ -44218,12 +44226,12 @@
       <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="53.453125" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="13.81640625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="18.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="11.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="53.44140625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="13.77734375" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="18.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="11.77734375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -44435,15 +44443,15 @@
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="39.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="11.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="14.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="14.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="16.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="17.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="18.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="39.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="11.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="14.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="14.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="16.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="17.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="18.21875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
@@ -44565,13 +44573,13 @@
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="25.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="25.5546875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="2" max="3" width="11" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="14.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="16.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="11.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="14.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="16.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="11.77734375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -44627,20 +44635,20 @@
       <selection activeCell="B22" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="26.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="88.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="26.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="88.44140625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="17" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="11.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="11.77734375" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="17" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="11.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="10" width="18.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="15.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="23.90625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="31.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="15.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="75.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="11.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="10" width="18.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="15.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="23.88671875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="31.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="15.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="75.5546875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17">
@@ -45345,20 +45353,20 @@
       <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="26.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="88.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="26.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="88.44140625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="17" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="11.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="11.77734375" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="17" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="11.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="10" width="18.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="15.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="23.90625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="31.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="15.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="75.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="11.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="10" width="18.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="15.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="23.88671875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="31.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="15.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="75.5546875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17">
@@ -45533,17 +45541,17 @@
       <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="109.81640625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="18.453125" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="39.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="109.77734375" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="18.44140625" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="39.21875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="4" max="4" width="15" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="30.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="34.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="18.1796875" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="16.81640625" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="16.1796875" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="30.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="34.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="18.21875" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="16.77734375" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="16.21875" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -45578,7 +45586,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="16.5">
+    <row r="2" spans="1:10" ht="16.8">
       <c r="A2" t="s">
         <v>1786</v>
       </c>
@@ -45720,21 +45728,21 @@
       <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="80.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="80.5546875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="11" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="16.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="16.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="15.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="21.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="14.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="9.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="14.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="21.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="16.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="16.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="15.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="21.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="14.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="9.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="14.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="21.77734375" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="15" max="15" width="16" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="14.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="14.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="14.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="14.77734375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18">
@@ -46255,72 +46263,72 @@
       <selection activeCell="BF8" sqref="BF8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="84.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="11.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="17.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="40.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="15.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="11.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="84.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="11.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="17.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="40.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="15.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="11.5546875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="7" max="7" width="13" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="15.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="12.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="15.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="12.44140625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="10" max="10" width="12" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="17.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="51.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="17.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="51.44140625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="13" max="13" width="15" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="10.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="11.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="3.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="15.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="17.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="28.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="23.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="18.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="28.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="25.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="24" max="24" width="12.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="25" max="25" width="3.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="10.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="11.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="3.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="15.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="17.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="28.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="23.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="18.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="28.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="25.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="12.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="25" max="25" width="3.77734375" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="26" max="26" width="7" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="27" max="27" width="9.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="28" max="28" width="17.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="29" max="29" width="5.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="9.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="28" max="28" width="17.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="29" max="29" width="5.5546875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="30" max="30" width="10" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="31" max="31" width="12.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="32" max="32" width="11.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="33" max="33" width="16.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="34" max="34" width="7.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="35" max="35" width="10.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="36" max="36" width="4.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="31" max="31" width="12.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="32" max="32" width="11.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="33" max="33" width="16.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="34" max="34" width="7.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="35" max="35" width="10.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="36" max="36" width="4.77734375" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="37" max="37" width="9" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="38" max="38" width="6.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="39" max="39" width="11.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="40" max="40" width="7.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="41" max="41" width="11.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="42" max="42" width="13.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="38" max="38" width="6.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="39" max="39" width="11.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="40" max="40" width="7.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="41" max="41" width="11.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="42" max="42" width="13.44140625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="43" max="43" width="14" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="44" max="44" width="13.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="45" max="45" width="7.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="46" max="46" width="13.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="44" max="44" width="13.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="45" max="45" width="7.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="46" max="46" width="13.21875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="48" max="48" width="10" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="49" max="49" width="5.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="50" max="50" width="6.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="51" max="51" width="7.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="52" max="52" width="9.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="53" max="53" width="10.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="54" max="54" width="14.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="49" max="49" width="5.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="50" max="50" width="6.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="51" max="51" width="7.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="52" max="52" width="9.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="53" max="53" width="10.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="54" max="54" width="14.77734375" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="55" max="55" width="20" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="56" max="56" width="8.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="57" max="57" width="8.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="58" max="60" width="19.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="61" max="61" width="12.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="62" max="62" width="10.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="63" max="63" width="24.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="64" max="64" width="15.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="65" max="65" width="24.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="66" max="66" width="16.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="67" max="67" width="5.81640625" customWidth="1" collapsed="1"/>
+    <col min="56" max="56" width="8.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="57" max="57" width="8.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="58" max="60" width="19.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="61" max="61" width="12.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="62" max="62" width="10.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="63" max="63" width="24.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="64" max="64" width="15.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="65" max="65" width="24.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="66" max="66" width="16.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="67" max="67" width="5.77734375" customWidth="1" collapsed="1"/>
     <col min="68" max="70" width="13" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
@@ -49319,15 +49327,15 @@
       <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="19.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="19.77734375" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="11" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="11.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="17.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="7.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="14.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="15.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="11.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="17.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="7.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="14.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="15.77734375" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="8" max="8" width="17" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
@@ -49396,26 +49404,26 @@
       <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="77.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="77.5546875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="11" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="12.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="14.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="20.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="12.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="14.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="20.5546875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="6" max="6" width="10" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="8" width="18.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="8" width="18.5546875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="9" max="9" width="18" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="10" max="10" width="19" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="21.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="8.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="15.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="11.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="16.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="20.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="16.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="21.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="8.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="15.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="11.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="16.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="20.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="16.77734375" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="18" max="18" width="16" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="13.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="13.21875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19">
@@ -50082,14 +50090,14 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="74" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="11.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="11.44140625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="11" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="4" max="4" width="13" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="9.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="10.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="9.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="10.21875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -50265,17 +50273,17 @@
       <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="113.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="113.21875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="11" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="11.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="14.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="6" width="9.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="11.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="14.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="6" width="9.77734375" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="7" max="7" width="17" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="11.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="10" width="17.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="38.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="11.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="10" width="17.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="38.5546875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
@@ -50467,19 +50475,19 @@
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="83.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="11.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="21.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="29.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="21.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="25.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="15.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="83.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="11.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="21.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="29.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="21.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="25.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="15.5546875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="8" max="8" width="11" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="197.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="10.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="19.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="197.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="10.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="19.77734375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
@@ -50776,20 +50784,20 @@
       <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="85.1796875" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="21.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="11.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="24.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="16.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="17.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="11.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="85.21875" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="21.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="11.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="24.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="16.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="17.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="11.77734375" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="8" max="8" width="11" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="33.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="8.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="28.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="15.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="33.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="8.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="28.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="15.5546875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
@@ -51832,9 +51840,9 @@
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="57.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="57.5546875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -51870,20 +51878,20 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="67.1796875" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="24.1796875" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="24.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="18.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="24.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="19.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="67.21875" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="24.21875" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="24.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="18.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="24.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="19.21875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="7" max="7" width="16" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="255.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="255.77734375" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="10" max="10" width="18" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="11.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="15.453125" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="25.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="11.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="15.44140625" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="25.77734375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16">
@@ -52500,9 +52508,9 @@
       <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="19.1796875" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="19.21875" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="79.54296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="79.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -52611,19 +52619,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2F00-000000000000}">
   <dimension ref="A1:AH9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="41.36328125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.36328125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.54296875" customWidth="1"/>
+    <col min="1" max="1" width="52.21875" customWidth="1"/>
+    <col min="6" max="6" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.5546875" customWidth="1"/>
     <col min="17" max="17" width="13" customWidth="1"/>
-    <col min="27" max="27" width="10.54296875" bestFit="1" customWidth="1"/>
-    <col min="31" max="33" width="12.6328125" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="19.6328125" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="31" max="33" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="19.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:34">
@@ -52721,7 +52730,7 @@
         <v>440</v>
       </c>
       <c r="AF1" s="11" t="s">
-        <v>1969</v>
+        <v>1968</v>
       </c>
       <c r="AG1" s="11" t="s">
         <v>441</v>
@@ -52825,7 +52834,7 @@
         <v>1958</v>
       </c>
       <c r="AF2" s="11" t="s">
-        <v>1970</v>
+        <v>1969</v>
       </c>
       <c r="AG2" s="11" t="s">
         <v>1958</v>
@@ -52929,7 +52938,7 @@
         <v>1958</v>
       </c>
       <c r="AF3" s="11" t="s">
-        <v>1970</v>
+        <v>1969</v>
       </c>
       <c r="AG3" s="11" t="s">
         <v>1958</v>
@@ -53033,7 +53042,7 @@
         <v>1958</v>
       </c>
       <c r="AF4" s="11" t="s">
-        <v>1970</v>
+        <v>1969</v>
       </c>
       <c r="AG4" s="11" t="s">
         <v>1958</v>
@@ -53137,7 +53146,7 @@
         <v>1958</v>
       </c>
       <c r="AF5" s="11" t="s">
-        <v>1970</v>
+        <v>1969</v>
       </c>
       <c r="AG5" s="11" t="s">
         <v>1958</v>
@@ -53148,7 +53157,7 @@
     </row>
     <row r="6" spans="1:34">
       <c r="A6" s="91" t="s">
-        <v>1968</v>
+        <v>1967</v>
       </c>
       <c r="B6" s="92" t="s">
         <v>106</v>
@@ -53241,7 +53250,7 @@
         <v>1966</v>
       </c>
       <c r="AF6" s="11" t="s">
-        <v>1970</v>
+        <v>1969</v>
       </c>
       <c r="AG6" s="11" t="s">
         <v>1966</v>
@@ -53252,7 +53261,7 @@
     </row>
     <row r="7" spans="1:34">
       <c r="A7" s="91" t="s">
-        <v>1967</v>
+        <v>1970</v>
       </c>
       <c r="B7" s="92" t="s">
         <v>106</v>
@@ -53270,7 +53279,7 @@
         <v>82</v>
       </c>
       <c r="G7" s="94" t="s">
-        <v>1950</v>
+        <v>1973</v>
       </c>
       <c r="H7" s="95" t="s">
         <v>24</v>
@@ -53336,7 +53345,7 @@
         <v>752</v>
       </c>
       <c r="AC7" s="93" t="s">
-        <v>1752</v>
+        <v>17</v>
       </c>
       <c r="AD7" s="93" t="s">
         <v>1752</v>
@@ -53345,7 +53354,7 @@
         <v>1958</v>
       </c>
       <c r="AF7" s="11" t="s">
-        <v>1970</v>
+        <v>1969</v>
       </c>
       <c r="AG7" s="11" t="s">
         <v>1958</v>
@@ -53355,8 +53364,8 @@
       </c>
     </row>
     <row r="8" spans="1:34">
-      <c r="A8" s="96" t="s">
-        <v>1971</v>
+      <c r="A8" s="91" t="s">
+        <v>1972</v>
       </c>
       <c r="B8" s="92" t="s">
         <v>106</v>
@@ -53374,7 +53383,7 @@
         <v>82</v>
       </c>
       <c r="G8" s="94" t="s">
-        <v>1950</v>
+        <v>1971</v>
       </c>
       <c r="H8" s="95" t="s">
         <v>24</v>
@@ -53434,7 +53443,7 @@
         <v>26</v>
       </c>
       <c r="AA8" s="93" t="s">
-        <v>1946</v>
+        <v>1944</v>
       </c>
       <c r="AB8" s="93" t="s">
         <v>1944</v>
@@ -53446,21 +53455,21 @@
         <v>1752</v>
       </c>
       <c r="AE8" s="11" t="s">
-        <v>224</v>
+        <v>1958</v>
       </c>
       <c r="AF8" s="11" t="s">
-        <v>1970</v>
+        <v>1969</v>
       </c>
       <c r="AG8" s="11" t="s">
-        <v>224</v>
+        <v>1958</v>
       </c>
       <c r="AH8" s="11" t="s">
         <v>1959</v>
       </c>
     </row>
     <row r="9" spans="1:34">
-      <c r="A9" s="96" t="s">
-        <v>1972</v>
+      <c r="A9" s="91" t="s">
+        <v>1975</v>
       </c>
       <c r="B9" s="92" t="s">
         <v>106</v>
@@ -53538,31 +53547,32 @@
         <v>26</v>
       </c>
       <c r="AA9" s="93" t="s">
-        <v>477</v>
+        <v>1946</v>
       </c>
       <c r="AB9" s="93" t="s">
-        <v>1946</v>
+        <v>1944</v>
       </c>
       <c r="AC9" s="93" t="s">
-        <v>1973</v>
+        <v>1752</v>
       </c>
       <c r="AD9" s="93" t="s">
-        <v>1973</v>
+        <v>1752</v>
       </c>
       <c r="AE9" s="11" t="s">
-        <v>224</v>
+        <v>1976</v>
       </c>
       <c r="AF9" s="11" t="s">
-        <v>1970</v>
+        <v>1969</v>
       </c>
       <c r="AG9" s="11" t="s">
-        <v>224</v>
+        <v>1976</v>
       </c>
       <c r="AH9" s="11" t="s">
-        <v>1959</v>
+        <v>1977</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -53572,79 +53582,79 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:BW35"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="78.453125" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="11.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="17.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="25.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="15.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="11.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="78.44140625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="11.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="17.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="25.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="15.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="11.5546875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="7" max="7" width="13" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="15.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="12.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="15.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="12.44140625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="10" max="10" width="12" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="17.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="15" width="17.1796875" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="17.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="15" width="17.21875" customWidth="1" collapsed="1"/>
     <col min="16" max="16" width="25" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="17.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="17.21875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="18" max="19" width="15" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="10.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="11.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="4.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="15.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="24" max="24" width="17.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="25" max="25" width="28.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="26" max="26" width="23.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="27" max="27" width="18.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="28" max="28" width="28.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="29" max="29" width="25.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="30" max="30" width="12.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="31" max="31" width="3.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="10.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="11.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="4.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="15.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="17.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="25" max="25" width="28.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="26" max="26" width="23.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="18.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="28" max="28" width="28.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="29" max="29" width="25.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="30" max="30" width="12.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="31" max="31" width="3.77734375" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="32" max="32" width="7" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="33" max="33" width="9.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="34" max="34" width="17.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="35" max="35" width="5.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="33" max="33" width="9.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="34" max="34" width="17.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="35" max="35" width="5.5546875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="36" max="36" width="10" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="37" max="37" width="12.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="38" max="38" width="11.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="39" max="39" width="16.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="40" max="40" width="7.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="41" max="41" width="10.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="42" max="42" width="4.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="37" max="37" width="12.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="38" max="38" width="11.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="39" max="39" width="16.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="40" max="40" width="7.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="41" max="41" width="10.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="42" max="42" width="4.77734375" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="43" max="43" width="9" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="44" max="44" width="6.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="45" max="45" width="11.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="46" max="46" width="7.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="47" max="47" width="11.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="48" max="48" width="13.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="44" max="44" width="6.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="45" max="45" width="11.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="46" max="46" width="7.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="47" max="47" width="11.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="48" max="48" width="13.44140625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="49" max="49" width="14" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="50" max="50" width="13.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="51" max="51" width="7.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="52" max="52" width="13.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="53" max="53" width="9.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="50" max="50" width="13.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="51" max="51" width="7.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="52" max="52" width="13.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="53" max="53" width="9.21875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="54" max="54" width="10" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="55" max="55" width="5.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="56" max="56" width="6.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="57" max="57" width="7.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="58" max="58" width="9.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="59" max="59" width="10.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="60" max="60" width="12.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="61" max="61" width="27.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="62" max="63" width="11.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="64" max="66" width="19.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="67" max="67" width="12.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="68" max="68" width="10.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="69" max="69" width="22.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="70" max="70" width="13.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="71" max="71" width="15.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="72" max="73" width="24.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="55" max="55" width="5.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="56" max="56" width="6.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="57" max="57" width="7.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="58" max="58" width="9.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="59" max="59" width="10.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="60" max="60" width="12.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="61" max="61" width="27.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="62" max="63" width="11.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="64" max="66" width="19.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="67" max="67" width="12.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="68" max="68" width="10.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="69" max="69" width="22.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="70" max="70" width="13.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="71" max="71" width="15.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="72" max="73" width="24.77734375" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="74" max="74" width="14" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="75" max="75" width="14.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="75" max="75" width="14.21875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:71">
@@ -54119,7 +54129,7 @@
       </c>
       <c r="N3" t="str">
         <f t="shared" ref="N3:N4" ca="1" si="0">CONCATENATE(E3," ",TEXT(TODAY(),"mm-dd-yyyy"))</f>
-        <v>SICA 09-15-2025</v>
+        <v>SICA 09-16-2025</v>
       </c>
       <c r="O3" t="s">
         <v>202</v>
@@ -54335,7 +54345,7 @@
       </c>
       <c r="N4" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>MICA 09-15-2025</v>
+        <v>MICA 09-16-2025</v>
       </c>
       <c r="O4" t="s">
         <v>202</v>
@@ -61220,7 +61230,7 @@
       <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
@@ -61245,15 +61255,15 @@
       <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="51.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="5" width="15.54296875" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="16.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="14.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="13.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="25.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="25.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="51.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="5" width="15.5546875" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="16.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="14.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="13.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="25.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="25.44140625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="16" max="16" width="22" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
@@ -61371,43 +61381,43 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="64" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="17.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="13.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="14.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="16.54296875" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="43.81640625" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="16.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="6.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="11.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="5.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="11.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="17.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="13.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="14.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="16.5546875" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="43.77734375" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="16.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="6.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="11.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="5.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="11.77734375" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="13" max="13" width="17" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="14" max="14" width="11" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="13.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="17" width="11.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="13.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="17" width="11.44140625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="18" max="18" width="15" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="13.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="11.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="21" max="23" width="13.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="25" max="25" width="11.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="26" max="26" width="57.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="27" max="27" width="19.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="28" max="28" width="18.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="29" max="29" width="25.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="30" max="30" width="9.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="31" max="31" width="11.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="32" max="32" width="36.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="33" max="33" width="31.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="34" max="34" width="16.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="13.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="11.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="23" width="13.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="25" max="25" width="11.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="26" max="26" width="57.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="19.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="28" max="28" width="18.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="29" max="29" width="25.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="30" max="30" width="9.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="31" max="31" width="11.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="32" max="32" width="36.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="33" max="33" width="31.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="34" max="34" width="16.77734375" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="35" max="35" width="14" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="36" max="36" width="14.81640625" customWidth="1" collapsed="1"/>
-    <col min="37" max="37" width="15.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="38" max="38" width="11.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="36" max="36" width="14.77734375" customWidth="1" collapsed="1"/>
+    <col min="37" max="37" width="15.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="38" max="38" width="11.5546875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="39" max="39" width="13" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="40" max="40" width="11.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="40" max="40" width="11.5546875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="41" max="41" width="13" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
@@ -62925,49 +62935,49 @@
       <selection activeCell="AN10" sqref="AN10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="35.453125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.81640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.1796875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.1796875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.81640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.81640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.81640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="6.81640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.81640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="6.54296875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.81640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.54296875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="18.1796875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="35.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.21875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.21875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.77734375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.77734375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.77734375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.77734375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.77734375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="6.5546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.77734375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="18.21875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.77734375" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="13" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="25.453125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="10.54296875" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="16.1796875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="14.1796875" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="11.1796875" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="10.1796875" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="11.1796875" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="14.453125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="25.44140625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="16.21875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="14.21875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="11.21875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="10.21875" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="11.21875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="14.44140625" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="11" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="9.1796875" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="18.54296875" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="20.81640625" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="19.453125" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="27.1796875" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="10.54296875" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="12.1796875" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="38.54296875" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="33.54296875" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="22.1796875" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="9.21875" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="18.5546875" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="20.77734375" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="19.44140625" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="27.21875" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="12.21875" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="38.5546875" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="33.5546875" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="22.21875" bestFit="1" customWidth="1"/>
     <col min="35" max="35" width="15" bestFit="1" customWidth="1"/>
     <col min="36" max="36" width="16" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="16.81640625" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="12.54296875" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="12.81640625" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="22.1796875" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="17.1796875" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="16.77734375" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="12.77734375" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="22.21875" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="17.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:41">
@@ -63351,26 +63361,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="0af65dbd-c349-4f95-a569-a37e7dcda261">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="a705add3-b55d-4a21-9da5-61558d9a88d9" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101004775ACE7CF61FD429C250F0EADD242CB" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="bdc0ef193019ef7ec3c6044774d719fd">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="0af65dbd-c349-4f95-a569-a37e7dcda261" xmlns:ns3="a705add3-b55d-4a21-9da5-61558d9a88d9" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="5eb62fd137b9132ea1ed680202856fff" ns2:_="" ns3:_="">
     <xsd:import namespace="0af65dbd-c349-4f95-a569-a37e7dcda261"/>
@@ -63625,26 +63615,27 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C7BF3F34-769C-4AFA-8719-29B8EDC91EB1}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4B56E0B5-42C8-48C9-A658-2E92FF4B9C74}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="0af65dbd-c349-4f95-a569-a37e7dcda261"/>
-    <ds:schemaRef ds:uri="a705add3-b55d-4a21-9da5-61558d9a88d9"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="0af65dbd-c349-4f95-a569-a37e7dcda261">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="a705add3-b55d-4a21-9da5-61558d9a88d9" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F2911B9E-6765-44F9-94CA-04166374824D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -63661,4 +63652,23 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C7BF3F34-769C-4AFA-8719-29B8EDC91EB1}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4B56E0B5-42C8-48C9-A658-2E92FF4B9C74}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="0af65dbd-c349-4f95-a569-a37e7dcda261"/>
+    <ds:schemaRef ds:uri="a705add3-b55d-4a21-9da5-61558d9a88d9"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>